<commit_message>
feat: eliminaciond de campos de mes y año redundantes para fechas ajuste visula del sidebar para texto blanco en modo oscuro
</commit_message>
<xml_diff>
--- a/backend/temp/SERVICIOS 2025.xlsx
+++ b/backend/temp/SERVICIOS 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481498b3c4373867/Documentos/DOCUMENTOS_EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2115" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{655F9A2E-A327-4BC2-964E-65DE366E0217}"/>
+  <xr:revisionPtr revIDLastSave="2129" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B457B0AA-9259-4EE1-98F0-D66EDBE42CBC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="6" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
   </bookViews>
@@ -26,28 +26,17 @@
     <sheet name="NOVIEMBRE" sheetId="11" r:id="rId11"/>
     <sheet name="DICIEMBRE" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1386" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="534">
   <si>
     <t>FECHA</t>
   </si>
@@ -1643,6 +1632,12 @@
   </si>
   <si>
     <t xml:space="preserve">revisión puerta vehicular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">cambio de fuente para tarjeta controladora de brazo electromecanico beninca 24v 10a ajsute y reprogemacion de parametros de apertura y cierre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">fuente 24v 10a </t>
   </si>
 </sst>
 </file>
@@ -19605,8 +19600,8 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView tabSelected="1" topLeftCell="I12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20090,7 +20085,7 @@
         <v>490</v>
       </c>
       <c r="G9" s="17">
-        <v>780000</v>
+        <v>740265</v>
       </c>
       <c r="H9" s="14" t="s">
         <v>491</v>
@@ -20107,18 +20102,18 @@
       </c>
       <c r="M9" s="6">
         <f t="shared" si="0"/>
-        <v>618000</v>
+        <v>578265</v>
       </c>
       <c r="N9" s="14" t="s">
         <v>21</v>
       </c>
       <c r="O9" s="6">
         <f t="shared" si="1"/>
-        <v>309000</v>
+        <v>289132.5</v>
       </c>
       <c r="P9" s="6">
         <f t="shared" si="2"/>
-        <v>457200</v>
+        <v>437332.5</v>
       </c>
       <c r="Q9" s="14" t="s">
         <v>50</v>
@@ -20657,32 +20652,56 @@
       <c r="R20" s="2"/>
       <c r="S20" s="14"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A21" s="2"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="14"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
+    <row r="21" spans="1:19" ht="58" x14ac:dyDescent="0.35">
+      <c r="A21" s="2">
+        <v>45868</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>519</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>520</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>532</v>
+      </c>
+      <c r="G21" s="17">
+        <v>807789</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>533</v>
+      </c>
+      <c r="I21" s="17">
+        <v>170000</v>
+      </c>
+      <c r="J21" s="17">
+        <v>161500</v>
+      </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="14"/>
+      <c r="L21" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M21" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="14"/>
-      <c r="O21" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>637789</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="6">
+        <f t="shared" si="1"/>
+        <v>318894.5</v>
       </c>
       <c r="P21" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q21" s="14"/>
+        <v>480394.5</v>
+      </c>
+      <c r="Q21" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="R21" s="2"/>
       <c r="S21" s="14"/>
     </row>

</xml_diff>

<commit_message>
Mejora visual y funcional del selector de meses: - Creado utils/dateFormatters.js para formatear nombres de meses y rangos de fechas - Creado utils/selectStyles.js para centralizar estilos del selector - Ajustado ServiciosPendientesEfectivo para usar formatearMesAnio y estilos personalizados - Orden correcto de meses en desplegables
</commit_message>
<xml_diff>
--- a/backend/temp/SERVICIOS 2025.xlsx
+++ b/backend/temp/SERVICIOS 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481498b3c4373867/Documentos/DOCUMENTOS_EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2129" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B457B0AA-9259-4EE1-98F0-D66EDBE42CBC}"/>
+  <xr:revisionPtr revIDLastSave="2192" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401C78CB-B5F2-4518-9E78-52E6DF37636E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="6" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="6" activeTab="7" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
   </bookViews>
   <sheets>
     <sheet name="ENERO" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="554">
   <si>
     <t>FECHA</t>
   </si>
@@ -1638,6 +1638,66 @@
   </si>
   <si>
     <t xml:space="preserve">fuente 24v 10a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jk envio desde nequi al nequi de jg </t>
+  </si>
+  <si>
+    <t>jk uso el 50% que le correspondia para cruzar con el pago del servicio de diag 60a # 22a - 66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">este servicio se cruza con el exedente que quedo debiendo jk en la relacion de los servicios que hubo confusion de lla diag 60a # 22a - 66 y dentix de suba donde se desconto mas de loque se le debia descontar a jg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALLE 101 # 13 - 41 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDIFICIO PORTAL DEL RINCÓN </t>
+  </si>
+  <si>
+    <t xml:space="preserve">desmonte ajuste y siliconado de zócalo inferior con Omar </t>
+  </si>
+  <si>
+    <t>jk hizo transferencia desde nequi al nequi jg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRA 46 # 18A - 36 - CANTON MILITAR CALDAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hernando Rodríguez </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESCUELA DE INGENIEROS </t>
+  </si>
+  <si>
+    <t>TRANSV 53A # 22 - 29 SUR</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>visita para cotizar mantenimiento puerta entrada vehicular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRA 53 # 5A - 65 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisión puerta entrada vehicular levadiza </t>
+  </si>
+  <si>
+    <t>CALLE 112 # 5A - 71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revision de motor de cremallera bft entrada vehicular </t>
+  </si>
+  <si>
+    <t xml:space="preserve">instalación de motor corredizo de cremallera bft entrada vehicular con JK </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jk hace transferencia desde la cuenta bancolombia al nequi de jg y deja la visita para la cotizacion como pago de la instalación </t>
+  </si>
+  <si>
+    <t xml:space="preserve">el valor que le corresponde a ABRECAR se deja como pago de la instalación del motor a jg </t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1861,7 @@
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="531">
+  <dxfs count="535">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1827,16 +1887,7 @@
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -1871,6 +1922,13 @@
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2519,16 +2577,127 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -2574,19 +2743,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2614,136 +2794,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -4227,7 +4299,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}" name="Tabla1" displayName="Tabla1" ref="A1:S41" totalsRowCount="1" headerRowDxfId="524" dataDxfId="523">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}" name="Tabla1" displayName="Tabla1" ref="A1:S41" totalsRowCount="1" headerRowDxfId="528" dataDxfId="527">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4250,38 +4322,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{88EFFA51-78C5-4D82-BB42-F4AEE89D019D}" name="FECHA" totalsRowLabel="Total" dataDxfId="522" totalsRowDxfId="521"/>
-    <tableColumn id="2" xr3:uid="{7B541160-E215-48CE-A708-A9B81341FB36}" name="DIRECCION" dataDxfId="520"/>
-    <tableColumn id="3" xr3:uid="{C87E6F99-2C33-41E1-910A-56118FB6CEA2}" name="NOMBRE CLIENTE" dataDxfId="519" totalsRowDxfId="518"/>
-    <tableColumn id="4" xr3:uid="{AC238300-B15A-40FF-BF70-F1ABBF4B84DB}" name="TORRE/APTO" dataDxfId="517" totalsRowDxfId="516"/>
-    <tableColumn id="5" xr3:uid="{DEBA4A69-A326-4346-9AF7-8F94C71F04B8}" name="SERVICIO REALIZADO" dataDxfId="515" totalsRowDxfId="514"/>
-    <tableColumn id="6" xr3:uid="{0C5C7083-E11A-4126-BB1C-58037F790853}" name="DOMICILIO" dataDxfId="513" totalsRowDxfId="512"/>
-    <tableColumn id="7" xr3:uid="{85C411DB-DD0C-4095-A483-1972E44C659E}" name="VALOR SERVICIO" dataDxfId="511" totalsRowDxfId="510"/>
-    <tableColumn id="8" xr3:uid="{BE982540-62B2-4C53-B539-D567DCB96001}" name="MATERIALES" dataDxfId="509"/>
-    <tableColumn id="9" xr3:uid="{D55AA2D8-3A08-47D0-9212-47CF0F007908}" name="VALOR MATERIALES" dataDxfId="508" totalsRowDxfId="507"/>
-    <tableColumn id="10" xr3:uid="{D05A4303-A355-4454-BCB2-EC086ADE67B7}" name="IVA 19%" dataDxfId="506" totalsRowDxfId="505"/>
-    <tableColumn id="11" xr3:uid="{668C804D-C86E-4B64-9768-E9C785F0DE00}" name="PORTERIA" dataDxfId="504" totalsRowDxfId="503"/>
-    <tableColumn id="12" xr3:uid="{46DB6D4C-9CC6-4252-96CF-72C1E3C46BEA}" name="FORMA DE PAGO " dataDxfId="502"/>
-    <tableColumn id="13" xr3:uid="{FA9B3154-D832-48D2-8D04-6729D9D451FA}" name="TOTAL SERVICIO" dataDxfId="501" totalsRowDxfId="500">
+    <tableColumn id="1" xr3:uid="{88EFFA51-78C5-4D82-BB42-F4AEE89D019D}" name="FECHA" totalsRowLabel="Total" dataDxfId="526" totalsRowDxfId="525"/>
+    <tableColumn id="2" xr3:uid="{7B541160-E215-48CE-A708-A9B81341FB36}" name="DIRECCION" dataDxfId="524"/>
+    <tableColumn id="3" xr3:uid="{C87E6F99-2C33-41E1-910A-56118FB6CEA2}" name="NOMBRE CLIENTE" dataDxfId="523" totalsRowDxfId="522"/>
+    <tableColumn id="4" xr3:uid="{AC238300-B15A-40FF-BF70-F1ABBF4B84DB}" name="TORRE/APTO" dataDxfId="521" totalsRowDxfId="520"/>
+    <tableColumn id="5" xr3:uid="{DEBA4A69-A326-4346-9AF7-8F94C71F04B8}" name="SERVICIO REALIZADO" dataDxfId="519" totalsRowDxfId="518"/>
+    <tableColumn id="6" xr3:uid="{0C5C7083-E11A-4126-BB1C-58037F790853}" name="DOMICILIO" dataDxfId="517" totalsRowDxfId="516"/>
+    <tableColumn id="7" xr3:uid="{85C411DB-DD0C-4095-A483-1972E44C659E}" name="VALOR SERVICIO" dataDxfId="515" totalsRowDxfId="514"/>
+    <tableColumn id="8" xr3:uid="{BE982540-62B2-4C53-B539-D567DCB96001}" name="MATERIALES" dataDxfId="513"/>
+    <tableColumn id="9" xr3:uid="{D55AA2D8-3A08-47D0-9212-47CF0F007908}" name="VALOR MATERIALES" dataDxfId="512" totalsRowDxfId="511"/>
+    <tableColumn id="10" xr3:uid="{D05A4303-A355-4454-BCB2-EC086ADE67B7}" name="IVA 19%" dataDxfId="510" totalsRowDxfId="509"/>
+    <tableColumn id="11" xr3:uid="{668C804D-C86E-4B64-9768-E9C785F0DE00}" name="PORTERIA" dataDxfId="508" totalsRowDxfId="507"/>
+    <tableColumn id="12" xr3:uid="{46DB6D4C-9CC6-4252-96CF-72C1E3C46BEA}" name="FORMA DE PAGO " dataDxfId="506"/>
+    <tableColumn id="13" xr3:uid="{FA9B3154-D832-48D2-8D04-6729D9D451FA}" name="TOTAL SERVICIO" dataDxfId="505" totalsRowDxfId="504">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{82B0E965-2F35-49F4-B770-9A98B3827FC7}" name="X50%/X25%" dataDxfId="499" totalsRowDxfId="498"/>
-    <tableColumn id="15" xr3:uid="{3E19AA37-CF0B-4C1B-B04A-0A62D3D17436}" name="PARA JG" dataDxfId="497" totalsRowDxfId="496">
+    <tableColumn id="14" xr3:uid="{82B0E965-2F35-49F4-B770-9A98B3827FC7}" name="X50%/X25%" dataDxfId="503" totalsRowDxfId="502"/>
+    <tableColumn id="15" xr3:uid="{3E19AA37-CF0B-4C1B-B04A-0A62D3D17436}" name="PARA JG" dataDxfId="501" totalsRowDxfId="500">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{2EB78162-0BC1-4664-A2A8-56110798321E}" name="PARA ABRECAR" dataDxfId="495" totalsRowDxfId="494">
+    <tableColumn id="16" xr3:uid="{2EB78162-0BC1-4664-A2A8-56110798321E}" name="PARA ABRECAR" dataDxfId="499" totalsRowDxfId="498">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{09F90FEF-782C-4AF1-B98E-46E81FF06B83}" name="ESTADO DEL SERVICIO" dataDxfId="493" totalsRowDxfId="492"/>
-    <tableColumn id="18" xr3:uid="{6BF05911-D79C-4CC7-98AF-584BCA918F60}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="491" totalsRowDxfId="490"/>
-    <tableColumn id="19" xr3:uid="{AC55681B-2B2C-491B-9108-650B648D57E8}" name="NOTAS " totalsRowFunction="count" dataDxfId="489"/>
+    <tableColumn id="17" xr3:uid="{09F90FEF-782C-4AF1-B98E-46E81FF06B83}" name="ESTADO DEL SERVICIO" dataDxfId="497" totalsRowDxfId="496"/>
+    <tableColumn id="18" xr3:uid="{6BF05911-D79C-4CC7-98AF-584BCA918F60}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="495" totalsRowDxfId="494"/>
+    <tableColumn id="19" xr3:uid="{AC55681B-2B2C-491B-9108-650B648D57E8}" name="NOTAS " totalsRowFunction="count" dataDxfId="493"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="120" dataDxfId="119">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4304,38 +4376,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="109"/>
-    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="108"/>
-    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="107"/>
-    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="106" totalsRowDxfId="105"/>
-    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="104"/>
-    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="103" totalsRowDxfId="102">
+    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="118" totalsRowDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="112" totalsRowDxfId="111" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="110" totalsRowDxfId="109"/>
+    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="108"/>
+    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="107"/>
+    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="106"/>
+    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="103"/>
+    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="102" totalsRowDxfId="101">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="99" totalsRowDxfId="98">
+    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="100" totalsRowDxfId="99"/>
+    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="98" totalsRowDxfId="97">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="97" totalsRowDxfId="96">
+    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="96" totalsRowDxfId="95">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="91"/>
+    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="94" totalsRowDxfId="93"/>
+    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="92" totalsRowDxfId="91"/>
+    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="83" dataDxfId="82">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4358,38 +4430,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="70"/>
-    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="66" totalsRowDxfId="65">
+    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="79"/>
+    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="77"/>
+    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="76"/>
+    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="75" totalsRowDxfId="74" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="71"/>
+    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="70"/>
+    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="69"/>
+    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="65" totalsRowDxfId="64">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="62" totalsRowDxfId="61">
+    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="61" totalsRowDxfId="60">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="59" totalsRowDxfId="58">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="53"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4412,38 +4484,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="38" totalsRowDxfId="37" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="28" totalsRowDxfId="27">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="24" totalsRowDxfId="23">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="22" totalsRowDxfId="21">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94438BA3-29D2-4F86-A312-A9854BED804A}" name="Tabla13" displayName="Tabla13" ref="A1:S41" totalsRowCount="1" headerRowDxfId="476" dataDxfId="475">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{94438BA3-29D2-4F86-A312-A9854BED804A}" name="Tabla13" displayName="Tabla13" ref="A1:S41" totalsRowCount="1" headerRowDxfId="480" dataDxfId="479">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4466,38 +4538,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{0D5AF355-292A-437A-ABFF-14D4EE864C29}" name="FECHA" totalsRowLabel="Total" dataDxfId="474" totalsRowDxfId="473"/>
-    <tableColumn id="2" xr3:uid="{5EA7179A-1A2E-4DA8-9CA0-A8CD4A717B15}" name="DIRECCION" dataDxfId="472" totalsRowDxfId="471"/>
-    <tableColumn id="3" xr3:uid="{E34E0C46-217A-438E-9B35-A0FF51FAC3F7}" name="NOMBRE CLIENTE" dataDxfId="470" totalsRowDxfId="469"/>
-    <tableColumn id="4" xr3:uid="{560F5D09-0B9E-4A04-A18C-BF23E3A80E5D}" name="TORRE/APTO" dataDxfId="468" totalsRowDxfId="467"/>
-    <tableColumn id="5" xr3:uid="{7134EEE2-6484-4F0E-9435-D17BB7E557CA}" name="SERVICIO REALIZADO" dataDxfId="466" totalsRowDxfId="465"/>
-    <tableColumn id="6" xr3:uid="{32BD03FE-E4E7-4E0E-B2A4-B633D6C0425A}" name="DOMICILIO" dataDxfId="464" totalsRowDxfId="463" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{44206A87-92DB-40AC-B414-3C66B7F4622D}" name="VALOR SERVICIO" dataDxfId="462" totalsRowDxfId="461"/>
-    <tableColumn id="8" xr3:uid="{14ABC623-5BB2-465D-A355-1E904638BB4F}" name="MATERIALES" dataDxfId="460" totalsRowDxfId="459"/>
-    <tableColumn id="9" xr3:uid="{BA6E9A66-ED27-4537-AFDE-7B52D7B2CFAD}" name="VALOR MATERIALES" dataDxfId="458" totalsRowDxfId="457"/>
-    <tableColumn id="10" xr3:uid="{F97C474D-0D87-427E-B496-3DD1D2D311BC}" name="IVA 19%" dataDxfId="456" totalsRowDxfId="455"/>
-    <tableColumn id="11" xr3:uid="{0569DB8A-2AA4-4706-85EA-49056986314D}" name="PORTERIA" dataDxfId="454" totalsRowDxfId="453"/>
-    <tableColumn id="12" xr3:uid="{CEA9ED83-3012-41AC-8AB2-F507C2E3B7FC}" name="FORMA DE PAGO " dataDxfId="452"/>
-    <tableColumn id="13" xr3:uid="{F52A621D-2C23-47B6-802B-1BEDE09C99C4}" name="TOTAL SERVICIO" dataDxfId="451" totalsRowDxfId="450">
+    <tableColumn id="1" xr3:uid="{0D5AF355-292A-437A-ABFF-14D4EE864C29}" name="FECHA" totalsRowLabel="Total" dataDxfId="478" totalsRowDxfId="477"/>
+    <tableColumn id="2" xr3:uid="{5EA7179A-1A2E-4DA8-9CA0-A8CD4A717B15}" name="DIRECCION" dataDxfId="476" totalsRowDxfId="475"/>
+    <tableColumn id="3" xr3:uid="{E34E0C46-217A-438E-9B35-A0FF51FAC3F7}" name="NOMBRE CLIENTE" dataDxfId="474" totalsRowDxfId="473"/>
+    <tableColumn id="4" xr3:uid="{560F5D09-0B9E-4A04-A18C-BF23E3A80E5D}" name="TORRE/APTO" dataDxfId="472" totalsRowDxfId="471"/>
+    <tableColumn id="5" xr3:uid="{7134EEE2-6484-4F0E-9435-D17BB7E557CA}" name="SERVICIO REALIZADO" dataDxfId="470" totalsRowDxfId="469"/>
+    <tableColumn id="6" xr3:uid="{32BD03FE-E4E7-4E0E-B2A4-B633D6C0425A}" name="DOMICILIO" dataDxfId="468" totalsRowDxfId="467" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{44206A87-92DB-40AC-B414-3C66B7F4622D}" name="VALOR SERVICIO" dataDxfId="466" totalsRowDxfId="465"/>
+    <tableColumn id="8" xr3:uid="{14ABC623-5BB2-465D-A355-1E904638BB4F}" name="MATERIALES" dataDxfId="464" totalsRowDxfId="463"/>
+    <tableColumn id="9" xr3:uid="{BA6E9A66-ED27-4537-AFDE-7B52D7B2CFAD}" name="VALOR MATERIALES" dataDxfId="462" totalsRowDxfId="461"/>
+    <tableColumn id="10" xr3:uid="{F97C474D-0D87-427E-B496-3DD1D2D311BC}" name="IVA 19%" dataDxfId="460" totalsRowDxfId="459"/>
+    <tableColumn id="11" xr3:uid="{0569DB8A-2AA4-4706-85EA-49056986314D}" name="PORTERIA" dataDxfId="458" totalsRowDxfId="457"/>
+    <tableColumn id="12" xr3:uid="{CEA9ED83-3012-41AC-8AB2-F507C2E3B7FC}" name="FORMA DE PAGO " dataDxfId="456"/>
+    <tableColumn id="13" xr3:uid="{F52A621D-2C23-47B6-802B-1BEDE09C99C4}" name="TOTAL SERVICIO" dataDxfId="455" totalsRowDxfId="454">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{5BAFF023-C8EE-4A74-B2B4-3CA0D6B08EE1}" name="X50%/X25%" dataDxfId="449" totalsRowDxfId="448"/>
-    <tableColumn id="15" xr3:uid="{844FBD5D-CD5B-4D22-817A-294B4EE3E163}" name="PARA JG" dataDxfId="447" totalsRowDxfId="446">
+    <tableColumn id="14" xr3:uid="{5BAFF023-C8EE-4A74-B2B4-3CA0D6B08EE1}" name="X50%/X25%" dataDxfId="453" totalsRowDxfId="452"/>
+    <tableColumn id="15" xr3:uid="{844FBD5D-CD5B-4D22-817A-294B4EE3E163}" name="PARA JG" dataDxfId="451" totalsRowDxfId="450">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{D4E47D5D-5691-4AD4-BAC3-4761D49930C8}" name="PARA ABRECAR" dataDxfId="445" totalsRowDxfId="444">
+    <tableColumn id="16" xr3:uid="{D4E47D5D-5691-4AD4-BAC3-4761D49930C8}" name="PARA ABRECAR" dataDxfId="449" totalsRowDxfId="448">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{73372BCF-EFFF-4EF5-814D-DFE11DDAB274}" name="ESTADO DEL SERVICIO" dataDxfId="443" totalsRowDxfId="442"/>
-    <tableColumn id="18" xr3:uid="{DD91CCFD-9DFE-47D4-940F-2D02FD2B7CE2}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="441" totalsRowDxfId="440"/>
-    <tableColumn id="19" xr3:uid="{BFD2664E-4D1B-4B0B-BC71-807C94F0E6FC}" name="NOTAS " totalsRowFunction="count" dataDxfId="439" totalsRowDxfId="438"/>
+    <tableColumn id="17" xr3:uid="{73372BCF-EFFF-4EF5-814D-DFE11DDAB274}" name="ESTADO DEL SERVICIO" dataDxfId="447" totalsRowDxfId="446"/>
+    <tableColumn id="18" xr3:uid="{DD91CCFD-9DFE-47D4-940F-2D02FD2B7CE2}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="445" totalsRowDxfId="444"/>
+    <tableColumn id="19" xr3:uid="{BFD2664E-4D1B-4B0B-BC71-807C94F0E6FC}" name="NOTAS " totalsRowFunction="count" dataDxfId="443" totalsRowDxfId="442"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EA784F1D-3DAA-4FF6-85B6-3A868655D2FD}" name="Tabla14" displayName="Tabla14" ref="A1:S41" totalsRowCount="1" headerRowDxfId="431" dataDxfId="430">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{EA784F1D-3DAA-4FF6-85B6-3A868655D2FD}" name="Tabla14" displayName="Tabla14" ref="A1:S41" totalsRowCount="1" headerRowDxfId="435" dataDxfId="434">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4520,38 +4592,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{D523D64C-D57B-4626-90E7-FD0731011868}" name="FECHA" totalsRowLabel="Total" dataDxfId="429" totalsRowDxfId="428"/>
-    <tableColumn id="2" xr3:uid="{147E84AE-230D-4E00-80B5-3E175839785C}" name="DIRECCION" dataDxfId="427"/>
-    <tableColumn id="3" xr3:uid="{3352E7E0-D480-4180-AA74-29C468449217}" name="NOMBRE CLIENTE" dataDxfId="426" totalsRowDxfId="425"/>
-    <tableColumn id="4" xr3:uid="{66F0647C-9F9F-44D6-B3DE-58982017DBD4}" name="TORRE/APTO" dataDxfId="424"/>
-    <tableColumn id="5" xr3:uid="{1FFB20B8-9F63-4AA2-B6BF-230DE6C71698}" name="SERVICIO REALIZADO" dataDxfId="423" totalsRowDxfId="422"/>
-    <tableColumn id="6" xr3:uid="{32435D80-CF43-4695-836B-3E9A2B56C146}" name="DOMICILIO" dataDxfId="421" totalsRowDxfId="420" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{85FD1E33-5A46-4C12-B448-BC9121DA9739}" name="VALOR SERVICIO" dataDxfId="419" totalsRowDxfId="418"/>
-    <tableColumn id="8" xr3:uid="{5D7C958E-4915-4369-8EB9-1E81282E2545}" name="MATERIALES" dataDxfId="417" totalsRowDxfId="416"/>
-    <tableColumn id="9" xr3:uid="{88473CBA-440F-41A0-BA4B-A67CE687D394}" name="VALOR MATERIALES" dataDxfId="415" totalsRowDxfId="414" dataCellStyle="Moneda"/>
-    <tableColumn id="10" xr3:uid="{953FDF9C-3ED4-41C5-BD3F-C7ADA7C18139}" name="IVA 19%" dataDxfId="413"/>
-    <tableColumn id="11" xr3:uid="{ECD176BE-4CE1-47E9-B4E5-6A846728A5AE}" name="PORTERIA" dataDxfId="412" totalsRowDxfId="411"/>
-    <tableColumn id="12" xr3:uid="{65743FE3-B63C-43CD-A2D4-E44B9380207A}" name="FORMA DE PAGO " dataDxfId="410"/>
-    <tableColumn id="13" xr3:uid="{2894C387-3068-4F17-A263-09DAF947A9A9}" name="TOTAL SERVICIO" dataDxfId="409" totalsRowDxfId="408">
+    <tableColumn id="1" xr3:uid="{D523D64C-D57B-4626-90E7-FD0731011868}" name="FECHA" totalsRowLabel="Total" dataDxfId="433" totalsRowDxfId="432"/>
+    <tableColumn id="2" xr3:uid="{147E84AE-230D-4E00-80B5-3E175839785C}" name="DIRECCION" dataDxfId="431"/>
+    <tableColumn id="3" xr3:uid="{3352E7E0-D480-4180-AA74-29C468449217}" name="NOMBRE CLIENTE" dataDxfId="430" totalsRowDxfId="429"/>
+    <tableColumn id="4" xr3:uid="{66F0647C-9F9F-44D6-B3DE-58982017DBD4}" name="TORRE/APTO" dataDxfId="428"/>
+    <tableColumn id="5" xr3:uid="{1FFB20B8-9F63-4AA2-B6BF-230DE6C71698}" name="SERVICIO REALIZADO" dataDxfId="427" totalsRowDxfId="426"/>
+    <tableColumn id="6" xr3:uid="{32435D80-CF43-4695-836B-3E9A2B56C146}" name="DOMICILIO" dataDxfId="425" totalsRowDxfId="424" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{85FD1E33-5A46-4C12-B448-BC9121DA9739}" name="VALOR SERVICIO" dataDxfId="423" totalsRowDxfId="422"/>
+    <tableColumn id="8" xr3:uid="{5D7C958E-4915-4369-8EB9-1E81282E2545}" name="MATERIALES" dataDxfId="421" totalsRowDxfId="420"/>
+    <tableColumn id="9" xr3:uid="{88473CBA-440F-41A0-BA4B-A67CE687D394}" name="VALOR MATERIALES" dataDxfId="419" totalsRowDxfId="418" dataCellStyle="Moneda"/>
+    <tableColumn id="10" xr3:uid="{953FDF9C-3ED4-41C5-BD3F-C7ADA7C18139}" name="IVA 19%" dataDxfId="417"/>
+    <tableColumn id="11" xr3:uid="{ECD176BE-4CE1-47E9-B4E5-6A846728A5AE}" name="PORTERIA" dataDxfId="416" totalsRowDxfId="415"/>
+    <tableColumn id="12" xr3:uid="{65743FE3-B63C-43CD-A2D4-E44B9380207A}" name="FORMA DE PAGO " dataDxfId="414"/>
+    <tableColumn id="13" xr3:uid="{2894C387-3068-4F17-A263-09DAF947A9A9}" name="TOTAL SERVICIO" dataDxfId="413" totalsRowDxfId="412">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{307F89ED-6745-41FB-97EA-3BECAD196C8B}" name="X50%/X25%" dataDxfId="407" totalsRowDxfId="406"/>
-    <tableColumn id="15" xr3:uid="{97E95D22-B758-46B9-9059-F746F1106DD4}" name="PARA JG" dataDxfId="405" totalsRowDxfId="404">
+    <tableColumn id="14" xr3:uid="{307F89ED-6745-41FB-97EA-3BECAD196C8B}" name="X50%/X25%" dataDxfId="411" totalsRowDxfId="410"/>
+    <tableColumn id="15" xr3:uid="{97E95D22-B758-46B9-9059-F746F1106DD4}" name="PARA JG" dataDxfId="409" totalsRowDxfId="408">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{2CB12610-BC89-41FE-96C4-CC02B13DF3BD}" name="PARA ABRECAR" dataDxfId="403" totalsRowDxfId="402">
+    <tableColumn id="16" xr3:uid="{2CB12610-BC89-41FE-96C4-CC02B13DF3BD}" name="PARA ABRECAR" dataDxfId="407" totalsRowDxfId="406">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{6E6D9331-E262-4A42-9E0B-5A30BF9A4281}" name="ESTADO DEL SERVICIO" dataDxfId="401" totalsRowDxfId="400"/>
-    <tableColumn id="18" xr3:uid="{5D266FF0-995F-4DA9-8CE3-15BE0BBF8702}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="399" totalsRowDxfId="398"/>
-    <tableColumn id="19" xr3:uid="{94DE83EA-515A-4C4F-83FD-17132BF224F6}" name="NOTAS " totalsRowFunction="count" dataDxfId="397" totalsRowDxfId="396"/>
+    <tableColumn id="17" xr3:uid="{6E6D9331-E262-4A42-9E0B-5A30BF9A4281}" name="ESTADO DEL SERVICIO" dataDxfId="405" totalsRowDxfId="404"/>
+    <tableColumn id="18" xr3:uid="{5D266FF0-995F-4DA9-8CE3-15BE0BBF8702}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="403" totalsRowDxfId="402"/>
+    <tableColumn id="19" xr3:uid="{94DE83EA-515A-4C4F-83FD-17132BF224F6}" name="NOTAS " totalsRowFunction="count" dataDxfId="401" totalsRowDxfId="400"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D539E001-6CC0-4E15-B866-F9D639064C10}" name="Tabla145" displayName="Tabla145" ref="A1:S41" totalsRowCount="1" headerRowDxfId="383" dataDxfId="382">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D539E001-6CC0-4E15-B866-F9D639064C10}" name="Tabla145" displayName="Tabla145" ref="A1:S41" totalsRowCount="1" headerRowDxfId="387" dataDxfId="386">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4574,38 +4646,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{ED00B034-A028-49EB-A74F-7B380E5CAEF6}" name="FECHA" totalsRowLabel="Total" dataDxfId="381" totalsRowDxfId="380"/>
-    <tableColumn id="2" xr3:uid="{56B21F16-EB7C-407B-9240-BA9C7E05EFB0}" name="DIRECCION" dataDxfId="379" totalsRowDxfId="378"/>
-    <tableColumn id="3" xr3:uid="{91C78E48-D4D3-4FFC-91C7-B42DFC7FD50C}" name="NOMBRE CLIENTE" dataDxfId="377" totalsRowDxfId="376"/>
-    <tableColumn id="4" xr3:uid="{31F67041-1F31-4308-8EC1-3DFBC27F3D0D}" name="TORRE/APTO" dataDxfId="375" totalsRowDxfId="374"/>
-    <tableColumn id="5" xr3:uid="{F5228A9C-D31D-4E94-A276-2378C2DAF53A}" name="SERVICIO REALIZADO" dataDxfId="373" totalsRowDxfId="372"/>
-    <tableColumn id="6" xr3:uid="{0307C712-1D29-4C68-80F4-DAC6765072D3}" name="DOMICILIO" dataDxfId="371" totalsRowDxfId="370" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{D8D9FF51-D262-4709-BD9C-E831827F7207}" name="VALOR SERVICIO" dataDxfId="369" totalsRowDxfId="368"/>
-    <tableColumn id="8" xr3:uid="{59E14D4C-867E-42B7-B9D3-3F182E31BFD0}" name="MATERIALES" dataDxfId="367"/>
-    <tableColumn id="9" xr3:uid="{F54B4CBC-743C-4A28-8FC4-AE9D671F04D0}" name="VALOR MATERIALES" dataDxfId="366" totalsRowDxfId="365"/>
-    <tableColumn id="10" xr3:uid="{A2DC869C-EAE2-496B-8CF2-A8139DBA2C83}" name="IVA 19%" dataDxfId="364" totalsRowDxfId="363"/>
-    <tableColumn id="11" xr3:uid="{9618C0AE-F9E6-4E83-A80E-51A561D98E94}" name="PORTERIA" dataDxfId="362" totalsRowDxfId="361"/>
-    <tableColumn id="12" xr3:uid="{EFF6D41C-F2CB-48D3-A8D3-D264EA27CBBA}" name="FORMA DE PAGO" dataDxfId="360"/>
-    <tableColumn id="13" xr3:uid="{A89B756E-94A8-47E8-84AD-90F416989867}" name="TOTAL SERVICIO" dataDxfId="359" totalsRowDxfId="358">
+    <tableColumn id="1" xr3:uid="{ED00B034-A028-49EB-A74F-7B380E5CAEF6}" name="FECHA" totalsRowLabel="Total" dataDxfId="385" totalsRowDxfId="384"/>
+    <tableColumn id="2" xr3:uid="{56B21F16-EB7C-407B-9240-BA9C7E05EFB0}" name="DIRECCION" dataDxfId="383" totalsRowDxfId="382"/>
+    <tableColumn id="3" xr3:uid="{91C78E48-D4D3-4FFC-91C7-B42DFC7FD50C}" name="NOMBRE CLIENTE" dataDxfId="381" totalsRowDxfId="380"/>
+    <tableColumn id="4" xr3:uid="{31F67041-1F31-4308-8EC1-3DFBC27F3D0D}" name="TORRE/APTO" dataDxfId="379" totalsRowDxfId="378"/>
+    <tableColumn id="5" xr3:uid="{F5228A9C-D31D-4E94-A276-2378C2DAF53A}" name="SERVICIO REALIZADO" dataDxfId="377" totalsRowDxfId="376"/>
+    <tableColumn id="6" xr3:uid="{0307C712-1D29-4C68-80F4-DAC6765072D3}" name="DOMICILIO" dataDxfId="375" totalsRowDxfId="374" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{D8D9FF51-D262-4709-BD9C-E831827F7207}" name="VALOR SERVICIO" dataDxfId="373" totalsRowDxfId="372"/>
+    <tableColumn id="8" xr3:uid="{59E14D4C-867E-42B7-B9D3-3F182E31BFD0}" name="MATERIALES" dataDxfId="371"/>
+    <tableColumn id="9" xr3:uid="{F54B4CBC-743C-4A28-8FC4-AE9D671F04D0}" name="VALOR MATERIALES" dataDxfId="370" totalsRowDxfId="369"/>
+    <tableColumn id="10" xr3:uid="{A2DC869C-EAE2-496B-8CF2-A8139DBA2C83}" name="IVA 19%" dataDxfId="368" totalsRowDxfId="367"/>
+    <tableColumn id="11" xr3:uid="{9618C0AE-F9E6-4E83-A80E-51A561D98E94}" name="PORTERIA" dataDxfId="366" totalsRowDxfId="365"/>
+    <tableColumn id="12" xr3:uid="{EFF6D41C-F2CB-48D3-A8D3-D264EA27CBBA}" name="FORMA DE PAGO" dataDxfId="364"/>
+    <tableColumn id="13" xr3:uid="{A89B756E-94A8-47E8-84AD-90F416989867}" name="TOTAL SERVICIO" dataDxfId="363" totalsRowDxfId="362">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{AE9135BF-0D6C-4959-A69E-3E5C5D042E28}" name="X50%/X25%" dataDxfId="357" totalsRowDxfId="356"/>
-    <tableColumn id="15" xr3:uid="{491B938F-932C-468D-86FC-2BBA0DA2DBE9}" name="PARA JG" dataDxfId="355" totalsRowDxfId="354">
+    <tableColumn id="14" xr3:uid="{AE9135BF-0D6C-4959-A69E-3E5C5D042E28}" name="X50%/X25%" dataDxfId="361" totalsRowDxfId="360"/>
+    <tableColumn id="15" xr3:uid="{491B938F-932C-468D-86FC-2BBA0DA2DBE9}" name="PARA JG" dataDxfId="359" totalsRowDxfId="358">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{D9977CB5-BC79-4024-846C-31F6F3A4CCFF}" name="PARA ABRECAR" dataDxfId="353" totalsRowDxfId="352">
+    <tableColumn id="16" xr3:uid="{D9977CB5-BC79-4024-846C-31F6F3A4CCFF}" name="PARA ABRECAR" dataDxfId="357" totalsRowDxfId="356">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{9B83594D-3936-4AF7-AFF5-DBC863A11601}" name="ESTADO DEL SERVICIO" dataDxfId="351" totalsRowDxfId="350"/>
-    <tableColumn id="18" xr3:uid="{9DBF688E-505C-4510-AD7C-F9790F220EDA}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="349" totalsRowDxfId="348"/>
-    <tableColumn id="19" xr3:uid="{309DC330-D156-42EE-8C7B-5CCA53126BD9}" name="NOTAS " totalsRowFunction="count" dataDxfId="347" totalsRowDxfId="346"/>
+    <tableColumn id="17" xr3:uid="{9B83594D-3936-4AF7-AFF5-DBC863A11601}" name="ESTADO DEL SERVICIO" dataDxfId="355" totalsRowDxfId="354"/>
+    <tableColumn id="18" xr3:uid="{9DBF688E-505C-4510-AD7C-F9790F220EDA}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="353" totalsRowDxfId="352"/>
+    <tableColumn id="19" xr3:uid="{309DC330-D156-42EE-8C7B-5CCA53126BD9}" name="NOTAS " totalsRowFunction="count" dataDxfId="351" totalsRowDxfId="350"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{79881273-217F-47F1-8A2C-EBBCB223955A}" name="Tabla1456" displayName="Tabla1456" ref="A1:S41" totalsRowCount="1" headerRowDxfId="309" dataDxfId="308">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{79881273-217F-47F1-8A2C-EBBCB223955A}" name="Tabla1456" displayName="Tabla1456" ref="A1:S41" totalsRowCount="1" headerRowDxfId="313" dataDxfId="312">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4628,38 +4700,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{0C3D997B-8408-42BF-B9C7-9515D4AE156B}" name="FECHA" totalsRowLabel="Total" dataDxfId="307" totalsRowDxfId="306"/>
-    <tableColumn id="2" xr3:uid="{6C918646-A8EB-433F-9FFD-93B416CB88FB}" name="DIRECCION" dataDxfId="305" totalsRowDxfId="304"/>
-    <tableColumn id="3" xr3:uid="{9F532EF3-F7D3-405B-AC54-2E37EEBA12E9}" name="NOMBRE CLIENTE" dataDxfId="303" totalsRowDxfId="302"/>
-    <tableColumn id="4" xr3:uid="{90648A10-62D5-431B-B3E5-B3DC6B0EB11F}" name="TORRE/APTO" dataDxfId="301"/>
-    <tableColumn id="5" xr3:uid="{AE19AAEF-9918-4095-B65A-D9AA41E7391D}" name="SERVICIO REALIZADO" dataDxfId="300" totalsRowDxfId="299"/>
-    <tableColumn id="6" xr3:uid="{DFBC4C92-256F-400E-9134-202E9652C8DF}" name="DOMICILIO" dataDxfId="298" totalsRowDxfId="297" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{6909FC11-08AC-4E7B-9C7A-87CC51E4258E}" name="VALOR SERVICIO" dataDxfId="296" totalsRowDxfId="295"/>
-    <tableColumn id="8" xr3:uid="{E376ADB2-7061-4F12-8B60-24E29AA1CA7E}" name="MATERIALES" dataDxfId="294"/>
-    <tableColumn id="9" xr3:uid="{02DE4204-9C5C-4CE3-A2C8-3344F0FFA0DF}" name="VALOR MATERIALES" dataDxfId="293" totalsRowDxfId="292"/>
-    <tableColumn id="10" xr3:uid="{122AE0D8-1F8F-45DB-AD40-9D3EB12570F7}" name="IVA 19%" dataDxfId="291" totalsRowDxfId="290"/>
-    <tableColumn id="11" xr3:uid="{7F9337DF-A066-47B1-BF46-BA371040214D}" name="PORTERIA" dataDxfId="289" totalsRowDxfId="288"/>
-    <tableColumn id="12" xr3:uid="{3CDD930A-C085-4794-95CA-22C887949175}" name="FORMA DE PAGO" dataDxfId="287"/>
-    <tableColumn id="13" xr3:uid="{F48495AF-F6C9-49C3-B2EF-37493691FD1F}" name="TOTAL SERVICIO" dataDxfId="286" totalsRowDxfId="285">
+    <tableColumn id="1" xr3:uid="{0C3D997B-8408-42BF-B9C7-9515D4AE156B}" name="FECHA" totalsRowLabel="Total" dataDxfId="311" totalsRowDxfId="310"/>
+    <tableColumn id="2" xr3:uid="{6C918646-A8EB-433F-9FFD-93B416CB88FB}" name="DIRECCION" dataDxfId="309" totalsRowDxfId="308"/>
+    <tableColumn id="3" xr3:uid="{9F532EF3-F7D3-405B-AC54-2E37EEBA12E9}" name="NOMBRE CLIENTE" dataDxfId="307" totalsRowDxfId="306"/>
+    <tableColumn id="4" xr3:uid="{90648A10-62D5-431B-B3E5-B3DC6B0EB11F}" name="TORRE/APTO" dataDxfId="305"/>
+    <tableColumn id="5" xr3:uid="{AE19AAEF-9918-4095-B65A-D9AA41E7391D}" name="SERVICIO REALIZADO" dataDxfId="304" totalsRowDxfId="303"/>
+    <tableColumn id="6" xr3:uid="{DFBC4C92-256F-400E-9134-202E9652C8DF}" name="DOMICILIO" dataDxfId="302" totalsRowDxfId="301" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{6909FC11-08AC-4E7B-9C7A-87CC51E4258E}" name="VALOR SERVICIO" dataDxfId="300" totalsRowDxfId="299"/>
+    <tableColumn id="8" xr3:uid="{E376ADB2-7061-4F12-8B60-24E29AA1CA7E}" name="MATERIALES" dataDxfId="298"/>
+    <tableColumn id="9" xr3:uid="{02DE4204-9C5C-4CE3-A2C8-3344F0FFA0DF}" name="VALOR MATERIALES" dataDxfId="297" totalsRowDxfId="296"/>
+    <tableColumn id="10" xr3:uid="{122AE0D8-1F8F-45DB-AD40-9D3EB12570F7}" name="IVA 19%" dataDxfId="295" totalsRowDxfId="294"/>
+    <tableColumn id="11" xr3:uid="{7F9337DF-A066-47B1-BF46-BA371040214D}" name="PORTERIA" dataDxfId="293" totalsRowDxfId="292"/>
+    <tableColumn id="12" xr3:uid="{3CDD930A-C085-4794-95CA-22C887949175}" name="FORMA DE PAGO" dataDxfId="291"/>
+    <tableColumn id="13" xr3:uid="{F48495AF-F6C9-49C3-B2EF-37493691FD1F}" name="TOTAL SERVICIO" dataDxfId="290" totalsRowDxfId="289">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{0E264A16-9366-478D-BFDA-A1EC5DEF28F8}" name="X50%/X25%" dataDxfId="284" totalsRowDxfId="283"/>
-    <tableColumn id="15" xr3:uid="{CDD3C1B0-7C9B-4B45-A89B-3E915E39435F}" name="PARA JG" dataDxfId="282" totalsRowDxfId="281">
+    <tableColumn id="14" xr3:uid="{0E264A16-9366-478D-BFDA-A1EC5DEF28F8}" name="X50%/X25%" dataDxfId="288" totalsRowDxfId="287"/>
+    <tableColumn id="15" xr3:uid="{CDD3C1B0-7C9B-4B45-A89B-3E915E39435F}" name="PARA JG" dataDxfId="286" totalsRowDxfId="285">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{174EF292-3C67-4C49-9A52-8FE4A18E7B12}" name="PARA ABRECAR" dataDxfId="280" totalsRowDxfId="279">
+    <tableColumn id="16" xr3:uid="{174EF292-3C67-4C49-9A52-8FE4A18E7B12}" name="PARA ABRECAR" dataDxfId="284" totalsRowDxfId="283">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{379B4F42-6BC6-41DE-81C7-5D50E0C5241A}" name="ESTADO DEL SERVICIO" dataDxfId="278" totalsRowDxfId="277"/>
-    <tableColumn id="18" xr3:uid="{1216CEED-DB81-4C1C-9006-3BC156C3217C}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="276" totalsRowDxfId="275"/>
-    <tableColumn id="19" xr3:uid="{75B8623C-4968-4E88-B6B7-5E69821F737F}" name="NOTAS " totalsRowFunction="count" dataDxfId="274" totalsRowDxfId="273"/>
+    <tableColumn id="17" xr3:uid="{379B4F42-6BC6-41DE-81C7-5D50E0C5241A}" name="ESTADO DEL SERVICIO" dataDxfId="282" totalsRowDxfId="281"/>
+    <tableColumn id="18" xr3:uid="{1216CEED-DB81-4C1C-9006-3BC156C3217C}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="280" totalsRowDxfId="279"/>
+    <tableColumn id="19" xr3:uid="{75B8623C-4968-4E88-B6B7-5E69821F737F}" name="NOTAS " totalsRowFunction="count" dataDxfId="278" totalsRowDxfId="277"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B846E70-E2BF-4CEF-B095-8D839C371C7F}" name="Tabla14567" displayName="Tabla14567" ref="A1:S42" totalsRowCount="1" headerRowDxfId="266" dataDxfId="265">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6B846E70-E2BF-4CEF-B095-8D839C371C7F}" name="Tabla14567" displayName="Tabla14567" ref="A1:S42" totalsRowCount="1" headerRowDxfId="270" dataDxfId="269">
   <autoFilter ref="A1:S41" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4682,38 +4754,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{714DB627-597B-40F5-8DE6-1DF144AE6820}" name="FECHA" totalsRowLabel="Total" dataDxfId="264" totalsRowDxfId="263"/>
-    <tableColumn id="2" xr3:uid="{88D21434-5D0F-4674-BDEE-8CC0788915A4}" name="DIRECCION" dataDxfId="262" totalsRowDxfId="261"/>
-    <tableColumn id="3" xr3:uid="{E32BD3E8-BF18-49DA-B123-76C0756BD1DA}" name="NOMBRE CLIENTE" dataDxfId="260" totalsRowDxfId="259"/>
-    <tableColumn id="4" xr3:uid="{3517C161-445C-4B3B-A68F-9A3C268787D3}" name="TORRE/APTO" dataDxfId="258"/>
-    <tableColumn id="5" xr3:uid="{C553111C-29C6-4403-BC45-908AAB0EC04A}" name="SERVICIO REALIZADO" dataDxfId="257" totalsRowDxfId="256"/>
-    <tableColumn id="6" xr3:uid="{DCE8AFCA-7869-4358-9104-4112D5020EC4}" name="DOMICILIO" dataDxfId="255" totalsRowDxfId="254" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{3F978537-BB51-40F4-A7F2-A73D8F8A934F}" name="VALOR SERVICIO" dataDxfId="253" totalsRowDxfId="252"/>
-    <tableColumn id="8" xr3:uid="{0A59C17C-D158-428B-8387-E0EDB61CB196}" name="MATERIALES" dataDxfId="251" totalsRowDxfId="250"/>
-    <tableColumn id="9" xr3:uid="{903BA4C8-A3C2-4E6F-BECE-BA4D82ED9611}" name="VALOR MATERIALES" dataDxfId="249" totalsRowDxfId="248"/>
-    <tableColumn id="10" xr3:uid="{B568D9A1-4F65-4F8C-BC98-5CE19A1E6002}" name="IVA 19%" dataDxfId="247" totalsRowDxfId="246"/>
-    <tableColumn id="11" xr3:uid="{9FD03442-E4B8-4F4A-8C4F-E0D085CBE3A2}" name="PORTERIA" dataDxfId="245" totalsRowDxfId="244"/>
-    <tableColumn id="12" xr3:uid="{60F0AE71-17A3-47C4-928E-B9444D1DEBB5}" name="FORMA DE PAGO " dataDxfId="243"/>
-    <tableColumn id="13" xr3:uid="{5E7335A0-FEF6-4BA1-9F7D-BE383E43CAAC}" name="TOTAL SERVICIO" dataDxfId="242" totalsRowDxfId="241">
+    <tableColumn id="1" xr3:uid="{714DB627-597B-40F5-8DE6-1DF144AE6820}" name="FECHA" totalsRowLabel="Total" dataDxfId="268" totalsRowDxfId="267"/>
+    <tableColumn id="2" xr3:uid="{88D21434-5D0F-4674-BDEE-8CC0788915A4}" name="DIRECCION" dataDxfId="266" totalsRowDxfId="265"/>
+    <tableColumn id="3" xr3:uid="{E32BD3E8-BF18-49DA-B123-76C0756BD1DA}" name="NOMBRE CLIENTE" dataDxfId="264" totalsRowDxfId="263"/>
+    <tableColumn id="4" xr3:uid="{3517C161-445C-4B3B-A68F-9A3C268787D3}" name="TORRE/APTO" dataDxfId="262"/>
+    <tableColumn id="5" xr3:uid="{C553111C-29C6-4403-BC45-908AAB0EC04A}" name="SERVICIO REALIZADO" dataDxfId="261" totalsRowDxfId="260"/>
+    <tableColumn id="6" xr3:uid="{DCE8AFCA-7869-4358-9104-4112D5020EC4}" name="DOMICILIO" dataDxfId="259" totalsRowDxfId="258" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{3F978537-BB51-40F4-A7F2-A73D8F8A934F}" name="VALOR SERVICIO" dataDxfId="257" totalsRowDxfId="256"/>
+    <tableColumn id="8" xr3:uid="{0A59C17C-D158-428B-8387-E0EDB61CB196}" name="MATERIALES" dataDxfId="255" totalsRowDxfId="254"/>
+    <tableColumn id="9" xr3:uid="{903BA4C8-A3C2-4E6F-BECE-BA4D82ED9611}" name="VALOR MATERIALES" dataDxfId="253" totalsRowDxfId="252"/>
+    <tableColumn id="10" xr3:uid="{B568D9A1-4F65-4F8C-BC98-5CE19A1E6002}" name="IVA 19%" dataDxfId="251" totalsRowDxfId="250"/>
+    <tableColumn id="11" xr3:uid="{9FD03442-E4B8-4F4A-8C4F-E0D085CBE3A2}" name="PORTERIA" dataDxfId="249" totalsRowDxfId="248"/>
+    <tableColumn id="12" xr3:uid="{60F0AE71-17A3-47C4-928E-B9444D1DEBB5}" name="FORMA DE PAGO " dataDxfId="247"/>
+    <tableColumn id="13" xr3:uid="{5E7335A0-FEF6-4BA1-9F7D-BE383E43CAAC}" name="TOTAL SERVICIO" dataDxfId="246" totalsRowDxfId="245">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A914A3D7-F0BB-4E54-9212-06F2668F4DFF}" name="X50%/X25%" dataDxfId="240" totalsRowDxfId="239"/>
-    <tableColumn id="15" xr3:uid="{5023FD9C-2775-4C44-9E67-4C241072F6BE}" name="PARA JG" dataDxfId="238" totalsRowDxfId="237">
+    <tableColumn id="14" xr3:uid="{A914A3D7-F0BB-4E54-9212-06F2668F4DFF}" name="X50%/X25%" dataDxfId="244" totalsRowDxfId="243"/>
+    <tableColumn id="15" xr3:uid="{5023FD9C-2775-4C44-9E67-4C241072F6BE}" name="PARA JG" dataDxfId="242" totalsRowDxfId="241">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{3CC141E2-AFA4-4913-BAED-ECA337F162B7}" name="PARA ABRECAR" dataDxfId="236" totalsRowDxfId="235">
+    <tableColumn id="16" xr3:uid="{3CC141E2-AFA4-4913-BAED-ECA337F162B7}" name="PARA ABRECAR" dataDxfId="240" totalsRowDxfId="239">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{1E630320-304C-437A-998F-E65910F1430C}" name="ESTADO DEL SERVICIO" dataDxfId="234" totalsRowDxfId="233"/>
-    <tableColumn id="18" xr3:uid="{00C6F989-EF5E-4069-B3D3-40B157EDE350}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="232" totalsRowDxfId="231"/>
-    <tableColumn id="19" xr3:uid="{744C0FA0-167F-4300-99A8-FFE7F1929262}" name="NOTAS " totalsRowFunction="count" dataDxfId="230" totalsRowDxfId="229"/>
+    <tableColumn id="17" xr3:uid="{1E630320-304C-437A-998F-E65910F1430C}" name="ESTADO DEL SERVICIO" dataDxfId="238" totalsRowDxfId="237"/>
+    <tableColumn id="18" xr3:uid="{00C6F989-EF5E-4069-B3D3-40B157EDE350}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="236" totalsRowDxfId="235"/>
+    <tableColumn id="19" xr3:uid="{744C0FA0-167F-4300-99A8-FFE7F1929262}" name="NOTAS " totalsRowFunction="count" dataDxfId="234" totalsRowDxfId="233"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4233D6D7-B829-4CFA-9D4A-3FA737BF65AA}" name="Tabla145678" displayName="Tabla145678" ref="A1:S41" totalsRowCount="1" headerRowDxfId="222" dataDxfId="221">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{4233D6D7-B829-4CFA-9D4A-3FA737BF65AA}" name="Tabla145678" displayName="Tabla145678" ref="A1:S41" totalsRowCount="1" headerRowDxfId="226" dataDxfId="225">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4736,38 +4808,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{E07C9A3C-C6D8-464B-8EF5-F396FABA9BE1}" name="FECHA" totalsRowLabel="Total" dataDxfId="220" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1A6A098E-D952-499C-96ED-9C233D840939}" name="DIRECCION" dataDxfId="219" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{D0010E5F-68B1-47A3-9F2E-4B18AEE9783B}" name="NOMBRE CLIENTE" dataDxfId="218" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{F76E2A6E-B436-49AB-AB58-87E162A07E6E}" name="TORRE/APTO" dataDxfId="217"/>
-    <tableColumn id="5" xr3:uid="{0AA2230E-5D5F-4272-A0DE-2F7507DFCB67}" name="SERVICIO REALIZADO" dataDxfId="216" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{F83C533A-63E6-47E8-B4E1-77C3349AE848}" name="DOMICILIO" dataDxfId="215" totalsRowDxfId="12" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{1C4F10E4-765A-4645-8374-D9F556D558D6}" name="VALOR SERVICIO" dataDxfId="214" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{38224342-79B1-43DE-8EEE-D0F522F52784}" name="MATERIALES" dataDxfId="213" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{2EB3AA1F-8E31-4F7D-A59E-7886D2D80133}" name="VALOR MATERIALES" dataDxfId="212" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{EDE45CFF-8F0A-4729-AC59-2F1A7E7E665B}" name="IVA 19%" dataDxfId="211" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{9F85F552-1AEA-4C75-B7BC-601D6ECE3576}" name="PORTERIA" dataDxfId="210" totalsRowDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{D94F26F3-BBDD-4540-B34F-A1931149813F}" name="FORMA DE PAGO " dataDxfId="209"/>
-    <tableColumn id="13" xr3:uid="{FD33B67F-7E7B-4AE3-83E7-03842134137F}" name="TOTAL SERVICIO" dataDxfId="208" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{E07C9A3C-C6D8-464B-8EF5-F396FABA9BE1}" name="FECHA" totalsRowLabel="Total" dataDxfId="224" totalsRowDxfId="223"/>
+    <tableColumn id="2" xr3:uid="{1A6A098E-D952-499C-96ED-9C233D840939}" name="DIRECCION" dataDxfId="222" totalsRowDxfId="221"/>
+    <tableColumn id="3" xr3:uid="{D0010E5F-68B1-47A3-9F2E-4B18AEE9783B}" name="NOMBRE CLIENTE" dataDxfId="220" totalsRowDxfId="219"/>
+    <tableColumn id="4" xr3:uid="{F76E2A6E-B436-49AB-AB58-87E162A07E6E}" name="TORRE/APTO" dataDxfId="218"/>
+    <tableColumn id="5" xr3:uid="{0AA2230E-5D5F-4272-A0DE-2F7507DFCB67}" name="SERVICIO REALIZADO" dataDxfId="217" totalsRowDxfId="216"/>
+    <tableColumn id="6" xr3:uid="{F83C533A-63E6-47E8-B4E1-77C3349AE848}" name="DOMICILIO" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{1C4F10E4-765A-4645-8374-D9F556D558D6}" name="VALOR SERVICIO" dataDxfId="213" totalsRowDxfId="212"/>
+    <tableColumn id="8" xr3:uid="{38224342-79B1-43DE-8EEE-D0F522F52784}" name="MATERIALES" dataDxfId="211" totalsRowDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{2EB3AA1F-8E31-4F7D-A59E-7886D2D80133}" name="VALOR MATERIALES" dataDxfId="209" totalsRowDxfId="208"/>
+    <tableColumn id="10" xr3:uid="{EDE45CFF-8F0A-4729-AC59-2F1A7E7E665B}" name="IVA 19%" dataDxfId="207" totalsRowDxfId="206"/>
+    <tableColumn id="11" xr3:uid="{9F85F552-1AEA-4C75-B7BC-601D6ECE3576}" name="PORTERIA" dataDxfId="205" totalsRowDxfId="204"/>
+    <tableColumn id="12" xr3:uid="{D94F26F3-BBDD-4540-B34F-A1931149813F}" name="FORMA DE PAGO " dataDxfId="203"/>
+    <tableColumn id="13" xr3:uid="{FD33B67F-7E7B-4AE3-83E7-03842134137F}" name="TOTAL SERVICIO" dataDxfId="202" totalsRowDxfId="201">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{574DE4C9-9D95-4D52-ACBB-99EA290AF592}" name="X50%/X25%" dataDxfId="207" totalsRowDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{19F5BE5D-091E-4103-A27C-7E02BB116F54}" name="PARA JG" dataDxfId="206" totalsRowDxfId="4">
+    <tableColumn id="14" xr3:uid="{574DE4C9-9D95-4D52-ACBB-99EA290AF592}" name="X50%/X25%" dataDxfId="200" totalsRowDxfId="199"/>
+    <tableColumn id="15" xr3:uid="{19F5BE5D-091E-4103-A27C-7E02BB116F54}" name="PARA JG" dataDxfId="198" totalsRowDxfId="197">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1F9C7C5-3D41-40E3-8489-1F206D47998D}" name="PARA ABRECAR" dataDxfId="205" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{F1F9C7C5-3D41-40E3-8489-1F206D47998D}" name="PARA ABRECAR" dataDxfId="196" totalsRowDxfId="195">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A390A234-094F-4D7C-AF12-820395FEDB2B}" name="ESTADO DEL SERVICIO" dataDxfId="204" totalsRowDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{02F7B8DC-4A83-4AD7-BFD1-7C44F4CAA839}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="203" totalsRowDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{26B7AF6C-079B-4277-96A6-4BFD38BF0059}" name="NOTAS " totalsRowFunction="count" dataDxfId="202" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{A390A234-094F-4D7C-AF12-820395FEDB2B}" name="ESTADO DEL SERVICIO" dataDxfId="194" totalsRowDxfId="193"/>
+    <tableColumn id="18" xr3:uid="{02F7B8DC-4A83-4AD7-BFD1-7C44F4CAA839}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="192" totalsRowDxfId="191"/>
+    <tableColumn id="19" xr3:uid="{26B7AF6C-079B-4277-96A6-4BFD38BF0059}" name="NOTAS " totalsRowFunction="count" dataDxfId="190" totalsRowDxfId="189"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{486570DD-72C3-4211-9F4B-38B695E2EB20}" name="Tabla1456789" displayName="Tabla1456789" ref="A1:S41" totalsRowCount="1" headerRowDxfId="195" dataDxfId="194">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{486570DD-72C3-4211-9F4B-38B695E2EB20}" name="Tabla1456789" displayName="Tabla1456789" ref="A1:S41" totalsRowCount="1" headerRowDxfId="182" dataDxfId="181">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4790,38 +4862,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3B888F1E-FD67-4F86-AA29-2A965EAFE3C4}" name="FECHA" totalsRowLabel="Total" dataDxfId="193" totalsRowDxfId="192"/>
-    <tableColumn id="2" xr3:uid="{7EF15A70-0B3B-4420-9167-C7DE9525619E}" name="DIRECCION" dataDxfId="191"/>
-    <tableColumn id="3" xr3:uid="{CF8A193F-3F32-495E-8083-92DCDAE2E9C4}" name="NOMBRE CLIENTE" dataDxfId="190"/>
-    <tableColumn id="4" xr3:uid="{D56B7752-FB26-4F5C-A7E4-ED5083929D15}" name="TORRE/APTO" dataDxfId="189"/>
-    <tableColumn id="5" xr3:uid="{B830E389-3B8E-41EB-ACE7-74A4840C91A9}" name="SERVICIO REALIZADO" dataDxfId="188"/>
-    <tableColumn id="6" xr3:uid="{4D7549D5-F072-4573-8E2F-F2B4062586CE}" name="DOMICILIO" dataDxfId="187" totalsRowDxfId="186" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{44BE91C0-C27A-4436-B0D9-494C81481BD9}" name="VALOR SERVICIO" dataDxfId="185" totalsRowDxfId="184"/>
-    <tableColumn id="8" xr3:uid="{E15FF744-2BD7-421C-9D41-D742D1B5FE8C}" name="MATERIALES" dataDxfId="183"/>
-    <tableColumn id="9" xr3:uid="{34230311-5EB0-4564-A8FF-85B470F2351F}" name="VALOR MATERIALES" dataDxfId="182"/>
-    <tableColumn id="10" xr3:uid="{A52B9B2D-6D58-41C4-9DAD-81D21868B2F4}" name="IVA 19%" dataDxfId="181"/>
-    <tableColumn id="11" xr3:uid="{E5CB6D2A-48AD-4BBE-89DD-DC2C080E54E3}" name="PORTERIA" dataDxfId="180" totalsRowDxfId="179"/>
-    <tableColumn id="12" xr3:uid="{5A3C93C6-6D8A-4CEC-9AD7-6622B5583AB4}" name="FORMA DE PAGO " dataDxfId="178"/>
-    <tableColumn id="13" xr3:uid="{D43E7292-D975-47ED-922A-20C879B75B71}" name="TOTAL SERVICIO" dataDxfId="177" totalsRowDxfId="176">
+    <tableColumn id="1" xr3:uid="{3B888F1E-FD67-4F86-AA29-2A965EAFE3C4}" name="FECHA" totalsRowLabel="Total" dataDxfId="180" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{7EF15A70-0B3B-4420-9167-C7DE9525619E}" name="DIRECCION" dataDxfId="179" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CF8A193F-3F32-495E-8083-92DCDAE2E9C4}" name="NOMBRE CLIENTE" dataDxfId="178"/>
+    <tableColumn id="4" xr3:uid="{D56B7752-FB26-4F5C-A7E4-ED5083929D15}" name="TORRE/APTO" dataDxfId="177" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{B830E389-3B8E-41EB-ACE7-74A4840C91A9}" name="SERVICIO REALIZADO" dataDxfId="176" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4D7549D5-F072-4573-8E2F-F2B4062586CE}" name="DOMICILIO" dataDxfId="175" totalsRowDxfId="9" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{44BE91C0-C27A-4436-B0D9-494C81481BD9}" name="VALOR SERVICIO" dataDxfId="174" totalsRowDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{E15FF744-2BD7-421C-9D41-D742D1B5FE8C}" name="MATERIALES" dataDxfId="173"/>
+    <tableColumn id="9" xr3:uid="{34230311-5EB0-4564-A8FF-85B470F2351F}" name="VALOR MATERIALES" dataDxfId="172"/>
+    <tableColumn id="10" xr3:uid="{A52B9B2D-6D58-41C4-9DAD-81D21868B2F4}" name="IVA 19%" dataDxfId="171"/>
+    <tableColumn id="11" xr3:uid="{E5CB6D2A-48AD-4BBE-89DD-DC2C080E54E3}" name="PORTERIA" dataDxfId="170" totalsRowDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{5A3C93C6-6D8A-4CEC-9AD7-6622B5583AB4}" name="FORMA DE PAGO " dataDxfId="169"/>
+    <tableColumn id="13" xr3:uid="{D43E7292-D975-47ED-922A-20C879B75B71}" name="TOTAL SERVICIO" dataDxfId="168" totalsRowDxfId="6">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A183837E-B67E-4FF9-B707-B5FB3439F80A}" name="X50%/X25%" dataDxfId="175" totalsRowDxfId="174"/>
-    <tableColumn id="15" xr3:uid="{686A4845-69ED-4068-9B0C-2A8D30EAE21C}" name="PARA JG" dataDxfId="173" totalsRowDxfId="172">
+    <tableColumn id="14" xr3:uid="{A183837E-B67E-4FF9-B707-B5FB3439F80A}" name="X50%/X25%" dataDxfId="167" totalsRowDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{686A4845-69ED-4068-9B0C-2A8D30EAE21C}" name="PARA JG" dataDxfId="166" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F8654BA2-147E-4B02-B8AD-A3ABCA9FD8B8}" name="PARA ABRECAR" dataDxfId="171" totalsRowDxfId="170">
+    <tableColumn id="16" xr3:uid="{F8654BA2-147E-4B02-B8AD-A3ABCA9FD8B8}" name="PARA ABRECAR" dataDxfId="165" totalsRowDxfId="3">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{4662DB30-1134-4599-9275-B92F7899D3ED}" name="ESTADO DEL SERVICIO" dataDxfId="169" totalsRowDxfId="168"/>
-    <tableColumn id="18" xr3:uid="{6542B359-24E7-4738-BCEA-B75973A57699}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="167" totalsRowDxfId="166"/>
-    <tableColumn id="19" xr3:uid="{A450A664-4EBD-4D5A-87FD-564564C00EDB}" name="NOTAS " totalsRowFunction="count" dataDxfId="165"/>
+    <tableColumn id="17" xr3:uid="{4662DB30-1134-4599-9275-B92F7899D3ED}" name="ESTADO DEL SERVICIO" dataDxfId="164" totalsRowDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{6542B359-24E7-4738-BCEA-B75973A57699}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{A450A664-4EBD-4D5A-87FD-564564C00EDB}" name="NOTAS " totalsRowFunction="count" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7D16E0DC-174B-4352-8C49-C57F1352E89E}" name="Tabla145678910" displayName="Tabla145678910" ref="A1:S41" totalsRowCount="1" headerRowDxfId="158" dataDxfId="157">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7D16E0DC-174B-4352-8C49-C57F1352E89E}" name="Tabla145678910" displayName="Tabla145678910" ref="A1:S41" totalsRowCount="1" headerRowDxfId="157" dataDxfId="156">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4844,31 +4916,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="156" totalsRowDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="153"/>
-    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="152"/>
-    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="151"/>
-    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="150" totalsRowDxfId="149" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="148" totalsRowDxfId="147"/>
-    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="146"/>
-    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="145"/>
-    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="144"/>
-    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="143" totalsRowDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="140" totalsRowDxfId="139">
+    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="155" totalsRowDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="152"/>
+    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="151"/>
+    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="150"/>
+    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="149" totalsRowDxfId="148" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="147" totalsRowDxfId="146"/>
+    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="145"/>
+    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="144"/>
+    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="143"/>
+    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="142" totalsRowDxfId="141"/>
+    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="140"/>
+    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="139" totalsRowDxfId="138">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="138" totalsRowDxfId="137"/>
-    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="136" totalsRowDxfId="135">
+    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="137" totalsRowDxfId="136"/>
+    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="135" totalsRowDxfId="134">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="134" totalsRowDxfId="133">
+    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="133" totalsRowDxfId="132">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="132" totalsRowDxfId="131"/>
-    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="130" totalsRowDxfId="129"/>
-    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="128"/>
+    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="127"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6896,22 +6968,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="530" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="534" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="529" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="533" priority="3" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="528" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="532" priority="4" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="527" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="531" priority="5" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="526" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="530" priority="6" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="525" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="529" priority="7" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8205,22 +8277,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="127" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9514,22 +9586,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="90" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10823,22 +10895,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="53" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12465,42 +12537,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S8 A9:R9 A10:S41">
-    <cfRule type="expression" dxfId="488" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="492" priority="7" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="487" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="491" priority="8" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="486" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="490" priority="9" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="485" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="489" priority="10" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="484" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="488" priority="11" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="483" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="487" priority="12" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="482" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="486" priority="1" stopIfTrue="1">
       <formula>$Q9="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="481" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="485" priority="2" stopIfTrue="1">
       <formula>$Q9="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="480" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="484" priority="3" stopIfTrue="1">
       <formula>$Q9="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="479" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="483" priority="4" stopIfTrue="1">
       <formula>$Q9="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="478" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="482" priority="5" stopIfTrue="1">
       <formula>$Q9="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="477" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="481" priority="6" stopIfTrue="1">
       <formula>$Q9="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13132,7 +13204,9 @@
       <c r="I12" s="27"/>
       <c r="J12" s="1"/>
       <c r="K12" s="6"/>
-      <c r="L12" s="14"/>
+      <c r="L12" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M12" s="6">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -13243,7 +13317,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="14" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="R14" s="31"/>
       <c r="S14" s="14"/>
@@ -14280,22 +14354,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="437" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="441" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="436" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="440" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="435" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="439" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="434" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="438" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="433" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="437" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="432" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="436" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15941,42 +16015,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S12 A13:R15 A16:S41">
-    <cfRule type="expression" dxfId="395" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="399" priority="19" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="394" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="398" priority="20" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="393" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="397" priority="21" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="392" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="396" priority="22" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="391" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="395" priority="23" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="390" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="394" priority="24" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13:S15">
-    <cfRule type="expression" dxfId="389" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="393" priority="1" stopIfTrue="1">
       <formula>$Q13="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="388" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="392" priority="2" stopIfTrue="1">
       <formula>$Q13="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="387" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="391" priority="3" stopIfTrue="1">
       <formula>$Q13="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="386" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="390" priority="4" stopIfTrue="1">
       <formula>$Q13="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="385" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="389" priority="5" stopIfTrue="1">
       <formula>$Q13="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="384" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="388" priority="6" stopIfTrue="1">
       <formula>$Q13="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17613,122 +17687,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="345" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="349" priority="36" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="344" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="348" priority="35" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="343" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="347" priority="34" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="342" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="346" priority="33" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="341" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="345" priority="32" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="340" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="344" priority="31" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="339" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="343" priority="19" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="338" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="342" priority="24" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="337" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="341" priority="23" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="336" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="340" priority="22" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="335" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="339" priority="21" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="334" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="338" priority="20" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="333" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="337" priority="13" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="332" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="336" priority="14" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="331" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="335" priority="15" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="330" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="334" priority="16" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="329" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="333" priority="17" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="328" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="332" priority="18" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 F2:S2 A3:S4 A5:R5 A6:S41">
-    <cfRule type="expression" dxfId="327" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="331" priority="42" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="326" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="330" priority="37" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="325" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="329" priority="38" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="324" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="328" priority="39" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="323" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="327" priority="40" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="322" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="326" priority="41" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="321" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="325" priority="12" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="320" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="324" priority="11" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="319" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="323" priority="10" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="318" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="322" priority="9" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="317" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="321" priority="8" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="316" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="320" priority="7" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="315" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="319" priority="6" stopIfTrue="1">
       <formula>$Q5="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="314" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="318" priority="5" stopIfTrue="1">
       <formula>$Q5="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="313" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="317" priority="4" stopIfTrue="1">
       <formula>$Q5="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="312" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="316" priority="3" stopIfTrue="1">
       <formula>$Q5="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="311" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="315" priority="2" stopIfTrue="1">
       <formula>$Q5="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="310" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="314" priority="1" stopIfTrue="1">
       <formula>$Q5="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17758,8 +17832,8 @@
   </sheetPr>
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18555,7 +18629,9 @@
       <c r="E15" s="14" t="s">
         <v>429</v>
       </c>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6">
+        <v>532000</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -18565,24 +18641,28 @@
       </c>
       <c r="M15" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>532000</v>
       </c>
       <c r="N15" s="14" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="6">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>133000</v>
       </c>
       <c r="P15" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>266000</v>
       </c>
       <c r="Q15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="R15" s="2">
+        <v>45835</v>
+      </c>
+      <c r="S15" s="14" t="s">
+        <v>540</v>
+      </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
@@ -19550,27 +19630,27 @@
       <c r="H42" s="15"/>
       <c r="S42" s="15">
         <f>SUBTOTAL(103,Tabla14567[[NOTAS ]])</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S42">
-    <cfRule type="expression" dxfId="272" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="276" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="271" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="275" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="270" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="274" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="269" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="273" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="268" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="272" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="267" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="271" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19600,8 +19680,8 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20116,10 +20196,14 @@
         <v>437332.5</v>
       </c>
       <c r="Q9" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="R9" s="2">
+        <v>45868</v>
+      </c>
+      <c r="S9" s="14" t="s">
+        <v>534</v>
+      </c>
     </row>
     <row r="10" spans="1:30" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
@@ -20511,9 +20595,15 @@
         <f t="shared" si="2"/>
         <v>40000</v>
       </c>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="14"/>
+      <c r="Q17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="2">
+        <v>45868</v>
+      </c>
+      <c r="S17" s="14" t="s">
+        <v>535</v>
+      </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
@@ -20563,7 +20653,7 @@
       <c r="R18" s="2"/>
       <c r="S18" s="14"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:19" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45866</v>
       </c>
@@ -20604,9 +20694,15 @@
         <f t="shared" si="2"/>
         <v>30000</v>
       </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="14"/>
+      <c r="Q19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R19" s="2">
+        <v>45868</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>536</v>
+      </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
@@ -20700,37 +20796,57 @@
         <v>480394.5</v>
       </c>
       <c r="Q21" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="R21" s="2"/>
-      <c r="S21" s="14"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="14"/>
+        <v>20</v>
+      </c>
+      <c r="R21" s="2">
+        <v>45868</v>
+      </c>
+      <c r="S21" s="14" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2">
+        <v>45869</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>537</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>538</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>539</v>
+      </c>
       <c r="G22" s="17"/>
       <c r="H22" s="14"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
       <c r="K22" s="6"/>
-      <c r="L22" s="14"/>
+      <c r="L22" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M22" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N22" s="14"/>
-      <c r="O22" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="N22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O22" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="P22" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="14"/>
+      <c r="Q22" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="R22" s="2"/>
       <c r="S22" s="14"/>
     </row>
@@ -21266,27 +21382,27 @@
       <c r="I41" s="18"/>
       <c r="S41" s="15">
         <f>SUBTOTAL(103,Tabla145678[[NOTAS ]])</f>
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="228" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="232" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="227" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="231" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="226" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="230" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="225" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="229" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="224" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="228" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="223" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="227" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21316,17 +21432,17 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" customWidth="1"/>
-    <col min="5" max="5" width="34.7265625" customWidth="1"/>
+    <col min="1" max="1" width="28" style="3" customWidth="1"/>
+    <col min="2" max="2" width="26.90625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="15" customWidth="1"/>
+    <col min="5" max="5" width="34.7265625" style="15" customWidth="1"/>
     <col min="6" max="6" width="17.08984375" style="7" customWidth="1"/>
     <col min="7" max="7" width="16.36328125" style="5" customWidth="1"/>
     <col min="8" max="8" width="39.54296875" customWidth="1"/>
@@ -21340,7 +21456,7 @@
     <col min="16" max="16" width="15.453125" style="10" customWidth="1"/>
     <col min="17" max="17" width="25.453125" style="12" customWidth="1"/>
     <col min="18" max="18" width="36.54296875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="47.6328125" customWidth="1"/>
+    <col min="19" max="19" width="65.1796875" style="15" customWidth="1"/>
     <col min="28" max="28" width="17.7265625" customWidth="1"/>
     <col min="29" max="29" width="26.36328125" customWidth="1"/>
   </cols>
@@ -21349,16 +21465,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="7" t="s">
@@ -21400,7 +21516,7 @@
       <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="14" t="s">
         <v>18</v>
       </c>
       <c r="AB1" s="1" t="s">
@@ -21413,34 +21529,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+    <row r="2" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>541</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>543</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="7">
+        <v>120000</v>
+      </c>
       <c r="G2" s="4"/>
       <c r="H2" s="1"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="L2" s="14"/>
+      <c r="L2" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M2" s="6">
         <f t="shared" ref="M2:M40" si="0">(F2+G2-I2-K2)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="6" t="str">
+        <v>120000</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="6">
         <f t="shared" ref="O2:O40" si="1">IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</f>
-        <v/>
+        <v>60000</v>
       </c>
       <c r="P2" s="6">
         <f t="shared" ref="P2:P40" si="2">(M2/2+J2)</f>
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="Q2" s="14"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="1"/>
+      <c r="S2" s="14"/>
       <c r="AB2" s="1" t="s">
         <v>26</v>
       </c>
@@ -21451,140 +21584,213 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+    <row r="3" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>45873</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>544</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="F3" s="7">
+        <v>80000</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="6"/>
-      <c r="L3" s="14"/>
+      <c r="L3" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M3" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N3" s="14"/>
-      <c r="O3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>80000</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="6">
+        <f t="shared" si="1"/>
+        <v>40000</v>
       </c>
       <c r="P3" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q3" s="14"/>
       <c r="R3" s="2"/>
-      <c r="S3" s="1"/>
+      <c r="S3" s="14"/>
       <c r="AC3" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>45873</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>547</v>
+      </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>548</v>
+      </c>
+      <c r="F4" s="7">
+        <v>80000</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="6"/>
-      <c r="L4" s="14"/>
+      <c r="L4" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M4" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N4" s="14"/>
-      <c r="O4" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>80000</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="6">
+        <f t="shared" si="1"/>
+        <v>40000</v>
       </c>
       <c r="P4" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q4" s="14"/>
       <c r="R4" s="2"/>
-      <c r="S4" s="1"/>
+      <c r="S4" s="14"/>
       <c r="AC4" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>45874</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>549</v>
+      </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>550</v>
+      </c>
+      <c r="F5" s="7">
+        <v>80000</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="6"/>
-      <c r="L5" s="14"/>
+      <c r="L5" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M5" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>80000</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="1"/>
+        <v>40000</v>
       </c>
       <c r="P5" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="1"/>
+        <v>40000</v>
+      </c>
+      <c r="Q5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R5" s="2">
+        <v>45875</v>
+      </c>
+      <c r="S5" s="14" t="s">
+        <v>553</v>
+      </c>
       <c r="AC5" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>45875</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>549</v>
+      </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="G6" s="4"/>
+      <c r="D6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>551</v>
+      </c>
+      <c r="G6" s="4">
+        <v>800000</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="14"/>
+      <c r="L6" s="14" t="s">
+        <v>19</v>
+      </c>
       <c r="M6" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N6" s="14"/>
-      <c r="O6" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>800000</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="6">
+        <f t="shared" si="1"/>
+        <v>400000</v>
       </c>
       <c r="P6" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="1"/>
+        <v>400000</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R6" s="2">
+        <v>45875</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>552</v>
+      </c>
       <c r="AC6" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
       <c r="G7" s="4"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -21606,17 +21812,17 @@
       </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="1"/>
+      <c r="S7" s="14"/>
       <c r="AC7" s="14" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="G8" s="4"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -21638,14 +21844,14 @@
       </c>
       <c r="Q8" s="14"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="1"/>
+      <c r="S8" s="14"/>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
       <c r="G9" s="4"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -21667,14 +21873,14 @@
       </c>
       <c r="Q9" s="14"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="1"/>
+      <c r="S9" s="14"/>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -21696,14 +21902,14 @@
       </c>
       <c r="Q10" s="14"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="1"/>
+      <c r="S10" s="14"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="14"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
       <c r="G11" s="4"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -21725,14 +21931,14 @@
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="1"/>
+      <c r="S11" s="14"/>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
       <c r="G12" s="4"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -21754,14 +21960,14 @@
       </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="1"/>
+      <c r="S12" s="14"/>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
-      <c r="B13" s="1"/>
+      <c r="B13" s="14"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
       <c r="G13" s="4"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -21783,14 +21989,14 @@
       </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="1"/>
+      <c r="S13" s="14"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
       <c r="G14" s="4"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -21812,14 +22018,14 @@
       </c>
       <c r="Q14" s="14"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="1"/>
+      <c r="S14" s="14"/>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
       <c r="G15" s="4"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -21841,14 +22047,14 @@
       </c>
       <c r="Q15" s="14"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="1"/>
+      <c r="S15" s="14"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
       <c r="G16" s="4"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -21870,14 +22076,14 @@
       </c>
       <c r="Q16" s="14"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="1"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
-      <c r="B17" s="1"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
       <c r="G17" s="4"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -21899,14 +22105,14 @@
       </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="1"/>
+      <c r="S17" s="14"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
       <c r="G18" s="4"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -21928,14 +22134,14 @@
       </c>
       <c r="Q18" s="14"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="1"/>
+      <c r="S18" s="14"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
       <c r="G19" s="4"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -21957,14 +22163,14 @@
       </c>
       <c r="Q19" s="14"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="1"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
-      <c r="B20" s="1"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
       <c r="G20" s="4"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -21986,14 +22192,14 @@
       </c>
       <c r="Q20" s="14"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="1"/>
+      <c r="S20" s="14"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="2"/>
-      <c r="B21" s="1"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
       <c r="G21" s="4"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -22015,14 +22221,14 @@
       </c>
       <c r="Q21" s="14"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="1"/>
+      <c r="S21" s="14"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
-      <c r="B22" s="1"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
       <c r="G22" s="4"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -22044,14 +22250,14 @@
       </c>
       <c r="Q22" s="14"/>
       <c r="R22" s="2"/>
-      <c r="S22" s="1"/>
+      <c r="S22" s="14"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
-      <c r="B23" s="1"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
       <c r="G23" s="4"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -22073,14 +22279,14 @@
       </c>
       <c r="Q23" s="14"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="1"/>
+      <c r="S23" s="14"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
       <c r="G24" s="4"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -22102,14 +22308,14 @@
       </c>
       <c r="Q24" s="14"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="14"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
       <c r="G25" s="4"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -22131,14 +22337,14 @@
       </c>
       <c r="Q25" s="14"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="1"/>
+      <c r="S25" s="14"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
-      <c r="B26" s="1"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
       <c r="G26" s="4"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -22160,14 +22366,14 @@
       </c>
       <c r="Q26" s="14"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="1"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="1"/>
+      <c r="B27" s="14"/>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
       <c r="G27" s="4"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -22189,14 +22395,14 @@
       </c>
       <c r="Q27" s="14"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="1"/>
+      <c r="S27" s="14"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
-      <c r="B28" s="1"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
       <c r="G28" s="4"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -22218,14 +22424,14 @@
       </c>
       <c r="Q28" s="14"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="1"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
-      <c r="B29" s="1"/>
+      <c r="B29" s="14"/>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
       <c r="G29" s="4"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -22247,14 +22453,14 @@
       </c>
       <c r="Q29" s="14"/>
       <c r="R29" s="2"/>
-      <c r="S29" s="1"/>
+      <c r="S29" s="14"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
-      <c r="B30" s="1"/>
+      <c r="B30" s="14"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
       <c r="G30" s="4"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -22276,14 +22482,14 @@
       </c>
       <c r="Q30" s="14"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="1"/>
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
-      <c r="B31" s="1"/>
+      <c r="B31" s="14"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
       <c r="G31" s="4"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -22305,14 +22511,14 @@
       </c>
       <c r="Q31" s="14"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="1"/>
+      <c r="S31" s="14"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
-      <c r="B32" s="1"/>
+      <c r="B32" s="14"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
       <c r="G32" s="4"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -22334,14 +22540,14 @@
       </c>
       <c r="Q32" s="14"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="1"/>
+      <c r="S32" s="14"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A33" s="2"/>
-      <c r="B33" s="1"/>
+      <c r="B33" s="14"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
       <c r="G33" s="4"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -22363,14 +22569,14 @@
       </c>
       <c r="Q33" s="14"/>
       <c r="R33" s="2"/>
-      <c r="S33" s="1"/>
+      <c r="S33" s="14"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A34" s="2"/>
-      <c r="B34" s="1"/>
+      <c r="B34" s="14"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
       <c r="G34" s="4"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -22392,14 +22598,14 @@
       </c>
       <c r="Q34" s="14"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="1"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="14"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
       <c r="G35" s="4"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -22421,14 +22627,14 @@
       </c>
       <c r="Q35" s="14"/>
       <c r="R35" s="2"/>
-      <c r="S35" s="1"/>
+      <c r="S35" s="14"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-      <c r="B36" s="1"/>
+      <c r="B36" s="14"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
       <c r="G36" s="4"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -22450,14 +22656,14 @@
       </c>
       <c r="Q36" s="14"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="1"/>
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
-      <c r="B37" s="1"/>
+      <c r="B37" s="14"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
       <c r="G37" s="4"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -22479,14 +22685,14 @@
       </c>
       <c r="Q37" s="14"/>
       <c r="R37" s="2"/>
-      <c r="S37" s="1"/>
+      <c r="S37" s="14"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
-      <c r="B38" s="1"/>
+      <c r="B38" s="14"/>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
       <c r="G38" s="4"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -22508,14 +22714,14 @@
       </c>
       <c r="Q38" s="14"/>
       <c r="R38" s="2"/>
-      <c r="S38" s="1"/>
+      <c r="S38" s="14"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
-      <c r="B39" s="1"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
       <c r="G39" s="4"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -22537,14 +22743,14 @@
       </c>
       <c r="Q39" s="14"/>
       <c r="R39" s="2"/>
-      <c r="S39" s="1"/>
+      <c r="S39" s="14"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
-      <c r="B40" s="1"/>
+      <c r="B40" s="14"/>
       <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
       <c r="G40" s="4"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -22566,36 +22772,36 @@
       </c>
       <c r="Q40" s="14"/>
       <c r="R40" s="2"/>
-      <c r="S40" s="1"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>120</v>
       </c>
       <c r="F41" s="13"/>
-      <c r="S41">
+      <c r="S41" s="15">
         <f>SUBTOTAL(103,Tabla1456789[[NOTAS ]])</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="201" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="188" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="200" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="187" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="199" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="186" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="198" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="185" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="197" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="184" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="196" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="183" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23889,22 +24095,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="164" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="163" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="162" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="162" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="161" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="161" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="160" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="159" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="158" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
♻️ Modularización de Analytics y mejoras UI - Modularización de Analytics en múltiples componentes (charts, tooltips, estados de carga/sin datos, sección KPI) - Creación de hook useAnalyticsData para centralizar lógica de datos - Sidebar: ítems de primer nivel ahora en negrita - KpiCard: soporte para valueStyle (ajuste dinámico de tamaño en valores) - Actualización de archivo Excel de pruebas
</commit_message>
<xml_diff>
--- a/backend/temp/SERVICIOS 2025.xlsx
+++ b/backend/temp/SERVICIOS 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481498b3c4373867/Documentos/DOCUMENTOS_EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2300" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD19F65C-365D-7145-B0AB-B559CDA82780}"/>
+  <xr:revisionPtr revIDLastSave="2320" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A1B5873-8715-B44C-8674-51D0DDB8FE2D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="7" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
   </bookViews>
   <sheets>
     <sheet name="ENERO" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="600">
   <si>
     <t>FECHA</t>
   </si>
@@ -1823,6 +1823,24 @@
   </si>
   <si>
     <t>jk pago desde nequi al nequi de jg</t>
+  </si>
+  <si>
+    <t>SEGURIDAD FENIX - Braheem Herrera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garantía de motor acces Matic instalado de jk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">jk paga $ 40.000 por arreglo que hizo jg el pago se toma del 50% de la CRA 12B # 10 - 23 sur  la visita de la  no se le cobra al cliente el poago lo asume jk </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRA 7 # 53 - 35 </t>
+  </si>
+  <si>
+    <t>EDIFICIO EL DORAL - Leonor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">revisión para instalar unidad de controles </t>
   </si>
 </sst>
 </file>
@@ -2012,16 +2030,10 @@
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
     <dxf>
       <font>
@@ -2053,6 +2065,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
@@ -3334,13 +3349,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -3348,6 +3357,86 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -3392,23 +3481,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3442,6 +3538,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3454,88 +3553,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -4485,7 +4503,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="223" dataDxfId="222">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="222" dataDxfId="221">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4508,38 +4526,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="221" totalsRowDxfId="220"/>
-    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="219"/>
-    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="218"/>
-    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="217"/>
-    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="216"/>
-    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="213" totalsRowDxfId="212"/>
-    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="211"/>
-    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="210"/>
-    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="209"/>
-    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="208" totalsRowDxfId="207"/>
-    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="206"/>
-    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="205" totalsRowDxfId="204">
+    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="220" totalsRowDxfId="219"/>
+    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="218"/>
+    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="217"/>
+    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="216"/>
+    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="215"/>
+    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="214" totalsRowDxfId="213" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="212" totalsRowDxfId="211"/>
+    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="210"/>
+    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="209"/>
+    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="208"/>
+    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="207" totalsRowDxfId="206"/>
+    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="205"/>
+    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="204" totalsRowDxfId="203">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="203" totalsRowDxfId="202"/>
-    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="201" totalsRowDxfId="200">
+    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="202" totalsRowDxfId="201"/>
+    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="200" totalsRowDxfId="199">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="199" totalsRowDxfId="198">
+    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="198" totalsRowDxfId="197">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="197" totalsRowDxfId="196"/>
-    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="195" totalsRowDxfId="194"/>
-    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="193"/>
+    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="196" totalsRowDxfId="195"/>
+    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="194" totalsRowDxfId="193"/>
+    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="192"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="192" dataDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="191" dataDxfId="190">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4562,38 +4580,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="190" totalsRowDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="188"/>
-    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="187"/>
-    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="186"/>
-    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="185"/>
-    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="184" totalsRowDxfId="183" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="182" totalsRowDxfId="181"/>
-    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="180"/>
-    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="179"/>
-    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="178"/>
-    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="177" totalsRowDxfId="176"/>
-    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="175"/>
-    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="174" totalsRowDxfId="173">
+    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="189" totalsRowDxfId="188"/>
+    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="187"/>
+    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="186"/>
+    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="185"/>
+    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="184"/>
+    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="183" totalsRowDxfId="182" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="181" totalsRowDxfId="180"/>
+    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="179"/>
+    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="178"/>
+    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="177"/>
+    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="176" totalsRowDxfId="175"/>
+    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="174"/>
+    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="173" totalsRowDxfId="172">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="172" totalsRowDxfId="171"/>
-    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="170" totalsRowDxfId="169">
+    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="171" totalsRowDxfId="170"/>
+    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="169" totalsRowDxfId="168">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="168" totalsRowDxfId="167">
+    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="167" totalsRowDxfId="166">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="166" totalsRowDxfId="165"/>
-    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="164" totalsRowDxfId="163"/>
-    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="162"/>
+    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="165" totalsRowDxfId="164"/>
+    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="163" totalsRowDxfId="162"/>
+    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="161"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="161" dataDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="160" dataDxfId="159">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4616,31 +4634,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="159" totalsRowDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="157"/>
-    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="156"/>
-    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="155"/>
-    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="154"/>
-    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="153" totalsRowDxfId="152" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="151" totalsRowDxfId="150"/>
-    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="149"/>
-    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="148"/>
-    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="147"/>
-    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="146" totalsRowDxfId="145"/>
-    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="144"/>
-    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="143" totalsRowDxfId="142">
+    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="158" totalsRowDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="156"/>
+    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="152" totalsRowDxfId="151" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="150" totalsRowDxfId="149"/>
+    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="148"/>
+    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="147"/>
+    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="146"/>
+    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="145" totalsRowDxfId="144"/>
+    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="143"/>
+    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="142" totalsRowDxfId="141">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="141" totalsRowDxfId="140"/>
-    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="139" totalsRowDxfId="138">
+    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="140" totalsRowDxfId="139"/>
+    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="138" totalsRowDxfId="137">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="137" totalsRowDxfId="136">
+    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="136" totalsRowDxfId="135">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="135" totalsRowDxfId="134"/>
-    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="133" totalsRowDxfId="132"/>
-    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="131"/>
+    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="134" totalsRowDxfId="133"/>
+    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="132" totalsRowDxfId="131"/>
+    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="130"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4940,38 +4958,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{E07C9A3C-C6D8-464B-8EF5-F396FABA9BE1}" name="FECHA" totalsRowLabel="Total" dataDxfId="310" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{1A6A098E-D952-499C-96ED-9C233D840939}" name="DIRECCION" dataDxfId="309" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{D0010E5F-68B1-47A3-9F2E-4B18AEE9783B}" name="NOMBRE CLIENTE" dataDxfId="308" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{F76E2A6E-B436-49AB-AB58-87E162A07E6E}" name="TORRE/APTO" dataDxfId="307"/>
-    <tableColumn id="5" xr3:uid="{0AA2230E-5D5F-4272-A0DE-2F7507DFCB67}" name="SERVICIO REALIZADO" dataDxfId="306" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{F83C533A-63E6-47E8-B4E1-77C3349AE848}" name="DOMICILIO" dataDxfId="305" totalsRowDxfId="12" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{1C4F10E4-765A-4645-8374-D9F556D558D6}" name="VALOR SERVICIO" dataDxfId="304" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{38224342-79B1-43DE-8EEE-D0F522F52784}" name="MATERIALES" dataDxfId="303" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{2EB3AA1F-8E31-4F7D-A59E-7886D2D80133}" name="VALOR MATERIALES" dataDxfId="302" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{EDE45CFF-8F0A-4729-AC59-2F1A7E7E665B}" name="IVA 19%" dataDxfId="301" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{9F85F552-1AEA-4C75-B7BC-601D6ECE3576}" name="PORTERIA" dataDxfId="300" totalsRowDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{D94F26F3-BBDD-4540-B34F-A1931149813F}" name="FORMA DE PAGO " dataDxfId="299"/>
-    <tableColumn id="13" xr3:uid="{FD33B67F-7E7B-4AE3-83E7-03842134137F}" name="TOTAL SERVICIO" dataDxfId="298" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{E07C9A3C-C6D8-464B-8EF5-F396FABA9BE1}" name="FECHA" totalsRowLabel="Total" dataDxfId="310" totalsRowDxfId="309"/>
+    <tableColumn id="2" xr3:uid="{1A6A098E-D952-499C-96ED-9C233D840939}" name="DIRECCION" dataDxfId="308" totalsRowDxfId="307"/>
+    <tableColumn id="3" xr3:uid="{D0010E5F-68B1-47A3-9F2E-4B18AEE9783B}" name="NOMBRE CLIENTE" dataDxfId="306" totalsRowDxfId="305"/>
+    <tableColumn id="4" xr3:uid="{F76E2A6E-B436-49AB-AB58-87E162A07E6E}" name="TORRE/APTO" dataDxfId="304"/>
+    <tableColumn id="5" xr3:uid="{0AA2230E-5D5F-4272-A0DE-2F7507DFCB67}" name="SERVICIO REALIZADO" dataDxfId="303" totalsRowDxfId="302"/>
+    <tableColumn id="6" xr3:uid="{F83C533A-63E6-47E8-B4E1-77C3349AE848}" name="DOMICILIO" dataDxfId="301" totalsRowDxfId="300" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{1C4F10E4-765A-4645-8374-D9F556D558D6}" name="VALOR SERVICIO" dataDxfId="299" totalsRowDxfId="298"/>
+    <tableColumn id="8" xr3:uid="{38224342-79B1-43DE-8EEE-D0F522F52784}" name="MATERIALES" dataDxfId="297" totalsRowDxfId="296"/>
+    <tableColumn id="9" xr3:uid="{2EB3AA1F-8E31-4F7D-A59E-7886D2D80133}" name="VALOR MATERIALES" dataDxfId="295" totalsRowDxfId="294"/>
+    <tableColumn id="10" xr3:uid="{EDE45CFF-8F0A-4729-AC59-2F1A7E7E665B}" name="IVA 19%" dataDxfId="293" totalsRowDxfId="292"/>
+    <tableColumn id="11" xr3:uid="{9F85F552-1AEA-4C75-B7BC-601D6ECE3576}" name="PORTERIA" dataDxfId="291" totalsRowDxfId="290"/>
+    <tableColumn id="12" xr3:uid="{D94F26F3-BBDD-4540-B34F-A1931149813F}" name="FORMA DE PAGO " dataDxfId="289"/>
+    <tableColumn id="13" xr3:uid="{FD33B67F-7E7B-4AE3-83E7-03842134137F}" name="TOTAL SERVICIO" dataDxfId="288" totalsRowDxfId="287">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{574DE4C9-9D95-4D52-ACBB-99EA290AF592}" name="X50%/X25%" dataDxfId="297" totalsRowDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{19F5BE5D-091E-4103-A27C-7E02BB116F54}" name="PARA JG" dataDxfId="296" totalsRowDxfId="4">
+    <tableColumn id="14" xr3:uid="{574DE4C9-9D95-4D52-ACBB-99EA290AF592}" name="X50%/X25%" dataDxfId="286" totalsRowDxfId="285"/>
+    <tableColumn id="15" xr3:uid="{19F5BE5D-091E-4103-A27C-7E02BB116F54}" name="PARA JG" dataDxfId="284" totalsRowDxfId="283">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F1F9C7C5-3D41-40E3-8489-1F206D47998D}" name="PARA ABRECAR" dataDxfId="295" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{F1F9C7C5-3D41-40E3-8489-1F206D47998D}" name="PARA ABRECAR" dataDxfId="282" totalsRowDxfId="281">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A390A234-094F-4D7C-AF12-820395FEDB2B}" name="ESTADO DEL SERVICIO" dataDxfId="294" totalsRowDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{02F7B8DC-4A83-4AD7-BFD1-7C44F4CAA839}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="293" totalsRowDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{26B7AF6C-079B-4277-96A6-4BFD38BF0059}" name="NOTAS " totalsRowFunction="count" dataDxfId="292" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{A390A234-094F-4D7C-AF12-820395FEDB2B}" name="ESTADO DEL SERVICIO" dataDxfId="280" totalsRowDxfId="279"/>
+    <tableColumn id="18" xr3:uid="{02F7B8DC-4A83-4AD7-BFD1-7C44F4CAA839}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="278" totalsRowDxfId="277"/>
+    <tableColumn id="19" xr3:uid="{26B7AF6C-079B-4277-96A6-4BFD38BF0059}" name="NOTAS " totalsRowFunction="count" dataDxfId="276" totalsRowDxfId="275"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{486570DD-72C3-4211-9F4B-38B695E2EB20}" name="Tabla1456789" displayName="Tabla1456789" ref="A1:S41" totalsRowCount="1" headerRowDxfId="291" dataDxfId="290">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{486570DD-72C3-4211-9F4B-38B695E2EB20}" name="Tabla1456789" displayName="Tabla1456789" ref="A1:S41" totalsRowCount="1" headerRowDxfId="274" dataDxfId="273">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4994,38 +5012,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3B888F1E-FD67-4F86-AA29-2A965EAFE3C4}" name="FECHA" totalsRowLabel="Total" dataDxfId="289" totalsRowDxfId="288"/>
-    <tableColumn id="2" xr3:uid="{7EF15A70-0B3B-4420-9167-C7DE9525619E}" name="DIRECCION" dataDxfId="287" totalsRowDxfId="286"/>
-    <tableColumn id="3" xr3:uid="{CF8A193F-3F32-495E-8083-92DCDAE2E9C4}" name="NOMBRE CLIENTE" dataDxfId="285" totalsRowDxfId="284"/>
-    <tableColumn id="4" xr3:uid="{D56B7752-FB26-4F5C-A7E4-ED5083929D15}" name="TORRE/APTO" dataDxfId="283" totalsRowDxfId="282"/>
-    <tableColumn id="5" xr3:uid="{B830E389-3B8E-41EB-ACE7-74A4840C91A9}" name="SERVICIO REALIZADO" dataDxfId="281" totalsRowDxfId="280"/>
-    <tableColumn id="6" xr3:uid="{4D7549D5-F072-4573-8E2F-F2B4062586CE}" name="DOMICILIO" dataDxfId="279" totalsRowDxfId="278" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{44BE91C0-C27A-4436-B0D9-494C81481BD9}" name="VALOR SERVICIO" dataDxfId="277" totalsRowDxfId="276"/>
-    <tableColumn id="8" xr3:uid="{E15FF744-2BD7-421C-9D41-D742D1B5FE8C}" name="MATERIALES" dataDxfId="275"/>
-    <tableColumn id="9" xr3:uid="{34230311-5EB0-4564-A8FF-85B470F2351F}" name="VALOR MATERIALES" dataDxfId="274" totalsRowDxfId="273"/>
-    <tableColumn id="10" xr3:uid="{A52B9B2D-6D58-41C4-9DAD-81D21868B2F4}" name="IVA 19%" dataDxfId="272"/>
-    <tableColumn id="11" xr3:uid="{E5CB6D2A-48AD-4BBE-89DD-DC2C080E54E3}" name="PORTERIA" dataDxfId="271" totalsRowDxfId="270"/>
-    <tableColumn id="12" xr3:uid="{5A3C93C6-6D8A-4CEC-9AD7-6622B5583AB4}" name="FORMA DE PAGO " dataDxfId="269"/>
-    <tableColumn id="13" xr3:uid="{D43E7292-D975-47ED-922A-20C879B75B71}" name="TOTAL SERVICIO" dataDxfId="268" totalsRowDxfId="267">
+    <tableColumn id="1" xr3:uid="{3B888F1E-FD67-4F86-AA29-2A965EAFE3C4}" name="FECHA" totalsRowLabel="Total" dataDxfId="272" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7EF15A70-0B3B-4420-9167-C7DE9525619E}" name="DIRECCION" dataDxfId="271" totalsRowDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CF8A193F-3F32-495E-8083-92DCDAE2E9C4}" name="NOMBRE CLIENTE" dataDxfId="270" totalsRowDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{D56B7752-FB26-4F5C-A7E4-ED5083929D15}" name="TORRE/APTO" dataDxfId="269" totalsRowDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{B830E389-3B8E-41EB-ACE7-74A4840C91A9}" name="SERVICIO REALIZADO" dataDxfId="268" totalsRowDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{4D7549D5-F072-4573-8E2F-F2B4062586CE}" name="DOMICILIO" dataDxfId="267" totalsRowDxfId="10" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{44BE91C0-C27A-4436-B0D9-494C81481BD9}" name="VALOR SERVICIO" dataDxfId="266" totalsRowDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{E15FF744-2BD7-421C-9D41-D742D1B5FE8C}" name="MATERIALES" dataDxfId="265"/>
+    <tableColumn id="9" xr3:uid="{34230311-5EB0-4564-A8FF-85B470F2351F}" name="VALOR MATERIALES" dataDxfId="264" totalsRowDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{A52B9B2D-6D58-41C4-9DAD-81D21868B2F4}" name="IVA 19%" dataDxfId="263"/>
+    <tableColumn id="11" xr3:uid="{E5CB6D2A-48AD-4BBE-89DD-DC2C080E54E3}" name="PORTERIA" dataDxfId="262" totalsRowDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{5A3C93C6-6D8A-4CEC-9AD7-6622B5583AB4}" name="FORMA DE PAGO " dataDxfId="261"/>
+    <tableColumn id="13" xr3:uid="{D43E7292-D975-47ED-922A-20C879B75B71}" name="TOTAL SERVICIO" dataDxfId="260" totalsRowDxfId="6">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{A183837E-B67E-4FF9-B707-B5FB3439F80A}" name="X50%/X25%" dataDxfId="266" totalsRowDxfId="265"/>
-    <tableColumn id="15" xr3:uid="{686A4845-69ED-4068-9B0C-2A8D30EAE21C}" name="PARA JG" dataDxfId="264" totalsRowDxfId="263">
+    <tableColumn id="14" xr3:uid="{A183837E-B67E-4FF9-B707-B5FB3439F80A}" name="X50%/X25%" dataDxfId="259" totalsRowDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{686A4845-69ED-4068-9B0C-2A8D30EAE21C}" name="PARA JG" dataDxfId="258" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F8654BA2-147E-4B02-B8AD-A3ABCA9FD8B8}" name="PARA ABRECAR" dataDxfId="262" totalsRowDxfId="261">
+    <tableColumn id="16" xr3:uid="{F8654BA2-147E-4B02-B8AD-A3ABCA9FD8B8}" name="PARA ABRECAR" dataDxfId="257" totalsRowDxfId="3">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{4662DB30-1134-4599-9275-B92F7899D3ED}" name="ESTADO DEL SERVICIO" dataDxfId="260" totalsRowDxfId="259"/>
-    <tableColumn id="18" xr3:uid="{6542B359-24E7-4738-BCEA-B75973A57699}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="258" totalsRowDxfId="257"/>
-    <tableColumn id="19" xr3:uid="{A450A664-4EBD-4D5A-87FD-564564C00EDB}" name="NOTAS " totalsRowFunction="count" dataDxfId="256" totalsRowDxfId="255"/>
+    <tableColumn id="17" xr3:uid="{4662DB30-1134-4599-9275-B92F7899D3ED}" name="ESTADO DEL SERVICIO" dataDxfId="256" totalsRowDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{6542B359-24E7-4738-BCEA-B75973A57699}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="255" totalsRowDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{A450A664-4EBD-4D5A-87FD-564564C00EDB}" name="NOTAS " totalsRowFunction="count" dataDxfId="254" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7D16E0DC-174B-4352-8C49-C57F1352E89E}" name="Tabla145678910" displayName="Tabla145678910" ref="A1:S41" totalsRowCount="1" headerRowDxfId="254" dataDxfId="253">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{7D16E0DC-174B-4352-8C49-C57F1352E89E}" name="Tabla145678910" displayName="Tabla145678910" ref="A1:S41" totalsRowCount="1" headerRowDxfId="253" dataDxfId="252">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5048,31 +5066,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="252" totalsRowDxfId="251"/>
-    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="250"/>
-    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="249"/>
-    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="248"/>
-    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="247"/>
-    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="246" totalsRowDxfId="245" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="244" totalsRowDxfId="243"/>
-    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="242"/>
-    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="241"/>
-    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="240"/>
-    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="239" totalsRowDxfId="238"/>
-    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="237"/>
-    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="236" totalsRowDxfId="235">
+    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="251" totalsRowDxfId="250"/>
+    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="249"/>
+    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="248"/>
+    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="247"/>
+    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="246"/>
+    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="245" totalsRowDxfId="244" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="243" totalsRowDxfId="242"/>
+    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="241"/>
+    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="240"/>
+    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="239"/>
+    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="238" totalsRowDxfId="237"/>
+    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="236"/>
+    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="235" totalsRowDxfId="234">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="234" totalsRowDxfId="233"/>
-    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="232" totalsRowDxfId="231">
+    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="233" totalsRowDxfId="232"/>
+    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="231" totalsRowDxfId="230">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="230" totalsRowDxfId="229">
+    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="229" totalsRowDxfId="228">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="228" totalsRowDxfId="227"/>
-    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="226" totalsRowDxfId="225"/>
-    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="224"/>
+    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="227" totalsRowDxfId="226"/>
+    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="225" totalsRowDxfId="224"/>
+    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="223"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7100,22 +7118,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="130" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="3" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="4" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="5" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="6" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="7" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8409,22 +8427,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="34" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9718,22 +9736,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="28" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11027,22 +11045,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="22" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12669,42 +12687,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S8 A9:R9 A10:S41">
-    <cfRule type="expression" dxfId="124" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="7" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="8" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="9" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="10" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="11" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="12" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S9">
-    <cfRule type="expression" dxfId="118" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="1" stopIfTrue="1">
       <formula>$Q9="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="2" stopIfTrue="1">
       <formula>$Q9="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="3" stopIfTrue="1">
       <formula>$Q9="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="114" priority="4" stopIfTrue="1">
       <formula>$Q9="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="113" priority="5" stopIfTrue="1">
       <formula>$Q9="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="112" priority="6" stopIfTrue="1">
       <formula>$Q9="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14498,22 +14516,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="112" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="111" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="107" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16163,42 +16181,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S12 A13:R15 A16:S41">
-    <cfRule type="expression" dxfId="106" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="19" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="20" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="21" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="22" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="23" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="24" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S13:S15">
-    <cfRule type="expression" dxfId="100" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="1" stopIfTrue="1">
       <formula>$Q13="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="2" stopIfTrue="1">
       <formula>$Q13="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="3" stopIfTrue="1">
       <formula>$Q13="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="97" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="4" stopIfTrue="1">
       <formula>$Q13="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="95" priority="5" stopIfTrue="1">
       <formula>$Q13="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="6" stopIfTrue="1">
       <formula>$Q13="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17845,122 +17863,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="94" priority="36" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="36" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="35" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="35" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="34" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="34" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="33" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="89" priority="32" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="31" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="expression" dxfId="88" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="19" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="24" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="23" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="22" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="21" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="20" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="82" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="13" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="14" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="15" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="16" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="17" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="18" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2 F2:S2 A3:S4 A5:R5 A6:S41">
-    <cfRule type="expression" dxfId="76" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="42" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="37" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="38" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="38" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="39" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="40" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="40" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="41" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="70" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="12" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="11" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="10" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="9" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="8" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="expression" dxfId="64" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="6" stopIfTrue="1">
       <formula>$Q5="CANCELADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="5" stopIfTrue="1">
       <formula>$Q5="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="4" stopIfTrue="1">
       <formula>$Q5="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="60" priority="3" stopIfTrue="1">
       <formula>$Q5="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="59" priority="2" stopIfTrue="1">
       <formula>$Q5="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="1" stopIfTrue="1">
       <formula>$Q5="YA RELACIONADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19793,22 +19811,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S42">
-    <cfRule type="expression" dxfId="58" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19838,7 +19856,7 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
@@ -21561,22 +21579,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="52" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21606,8 +21624,8 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22406,64 +22424,98 @@
       <c r="E17" s="14" t="s">
         <v>589</v>
       </c>
+      <c r="F17" s="7">
+        <v>80000</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="1"/>
       <c r="I17" s="6"/>
       <c r="J17" s="1"/>
       <c r="K17" s="6"/>
-      <c r="L17" s="14"/>
+      <c r="L17" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M17" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N17" s="14"/>
-      <c r="O17" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>80000</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="6">
+        <f t="shared" si="1"/>
+        <v>40000</v>
       </c>
       <c r="P17" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q17" s="14"/>
       <c r="R17" s="2"/>
       <c r="S17" s="14"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
+    <row r="18" spans="1:19" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>45890</v>
+      </c>
       <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="C18" s="14" t="s">
+        <v>592</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>593</v>
+      </c>
+      <c r="F18" s="7">
+        <v>80000</v>
+      </c>
       <c r="G18" s="6"/>
       <c r="H18" s="1"/>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
       <c r="K18" s="6"/>
-      <c r="L18" s="14"/>
+      <c r="L18" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M18" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="14"/>
-      <c r="O18" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>80000</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="6">
+        <f t="shared" si="1"/>
+        <v>40000</v>
       </c>
       <c r="P18" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q18" s="14"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="14"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="S18" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="27.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>45891</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>595</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>596</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>557</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>597</v>
+      </c>
       <c r="G19" s="6"/>
       <c r="H19" s="1"/>
       <c r="I19" s="6"/>
@@ -22483,7 +22535,9 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q19" s="14"/>
+      <c r="Q19" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="R19" s="2"/>
       <c r="S19" s="14"/>
     </row>
@@ -23103,27 +23157,27 @@
       <c r="F41" s="13"/>
       <c r="S41" s="15">
         <f>SUBTOTAL(103,Tabla1456789[[NOTAS ]])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="46" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24417,22 +24471,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="40" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
cambiio de archivo .env
</commit_message>
<xml_diff>
--- a/backend/temp/SERVICIOS 2025.xlsx
+++ b/backend/temp/SERVICIOS 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/481498B3C4373867/DOCUMENTOS_EXCEL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2578" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CDA4F68-BB81-4FE5-AEDB-F6B483EC049E}"/>
+  <xr:revisionPtr revIDLastSave="2586" documentId="8_{FFC92CA8-A633-40BE-8E56-4F9D61ABD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F790C3A8-7746-9B46-9B0D-E3B224C3EDF2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="8" xr2:uid="{58C13FB9-58C5-4D53-86A7-FA1AAB49DCCE}"/>
   </bookViews>
@@ -26,10 +26,21 @@
     <sheet name="NOVIEMBRE" sheetId="11" r:id="rId11"/>
     <sheet name="DICIEMBRE" sheetId="13" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
@@ -39,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1664" uniqueCount="674">
   <si>
     <t>FECHA</t>
   </si>
@@ -2052,6 +2063,15 @@
   </si>
   <si>
     <t>JG  hace transferencia de $185.600 para copletar el pago del servicio a ABRECAR el cliente ya le habia abonado $450.000 este pago incluye los $60.000 de la bateria y la caja que se tomaron de la oficina y los $40.000 de la visita inicial se hizo por transferencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALLE 23 SUR # 6 - 31 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yamcar Carlos Díaz </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajuste de puertas de vidrio corredizas entrada y chapa mantenimiento </t>
   </si>
 </sst>
 </file>
@@ -2217,40 +2237,75 @@
   </cellStyles>
   <dxfs count="546">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2273,16 +2328,75 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2609,7 +2723,10 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -2664,19 +2781,30 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2704,136 +2832,28 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="[$$-540A]#,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="&quot;$&quot;\ #,##0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -4744,7 +4764,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{D3DC7B56-6A27-47EA-8A62-6146CB27CD41}" name="Tabla14567891011" displayName="Tabla14567891011" ref="A1:S41" totalsRowCount="1" headerRowDxfId="104" dataDxfId="103">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4767,38 +4787,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="119" totalsRowDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="113" totalsRowDxfId="112" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="109"/>
-    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="108"/>
-    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="107"/>
-    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="106" totalsRowDxfId="105"/>
-    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="104"/>
-    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="103" totalsRowDxfId="102">
+    <tableColumn id="1" xr3:uid="{94F08EE5-D270-4BBA-BFF0-760C6EE7067B}" name="FECHA" totalsRowLabel="Total" dataDxfId="102" totalsRowDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{4C53B68C-163E-46DC-B529-42A48BCB11F4}" name="DIRECCION" dataDxfId="100"/>
+    <tableColumn id="3" xr3:uid="{79BD3134-74F1-4163-BEA0-1250C669D816}" name="NOMBRE CLIENTE" dataDxfId="99"/>
+    <tableColumn id="4" xr3:uid="{9B7351AF-69A8-42A0-88CF-7F1D324558CD}" name="TORRE/APTO" dataDxfId="98"/>
+    <tableColumn id="5" xr3:uid="{3FC795B0-64D5-412F-967D-88FDCE6188CC}" name="SERVICIO REALIZADO" dataDxfId="97"/>
+    <tableColumn id="6" xr3:uid="{F8E4C084-C1E1-410A-9AB8-48E3E1C03449}" name="DOMICILIO" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{3923866B-5E04-4E69-B31A-D524F1DB0AAC}" name="VALOR SERVICIO" dataDxfId="94" totalsRowDxfId="93"/>
+    <tableColumn id="8" xr3:uid="{8D9C03FA-D5F4-4C9D-B0D6-0B3FE724EB6D}" name="MATERIALES" dataDxfId="92"/>
+    <tableColumn id="9" xr3:uid="{416A2E87-138A-49CF-B9F5-D318A063AD9F}" name="VALOR MATERIALES" dataDxfId="91"/>
+    <tableColumn id="10" xr3:uid="{A82F5C41-8889-4BC2-8CD0-E17F28FC8B69}" name="IVA 19%" dataDxfId="90"/>
+    <tableColumn id="11" xr3:uid="{8AE9AA77-4CCE-4933-9E37-2424517466ED}" name="PORTERIA" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{9AEF8C4D-8BF9-4E7D-B1C4-77744EC693C7}" name="FORMA DE PAGO " dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{E6A473EB-A02F-4383-8D91-3F21721D15F3}" name="TOTAL SERVICIO" dataDxfId="86" totalsRowDxfId="85">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="99" totalsRowDxfId="98">
+    <tableColumn id="14" xr3:uid="{D278A045-9615-406B-B68A-49A1BAA68123}" name="X50%/X25%" dataDxfId="84" totalsRowDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{27DD6F2B-55CE-4F91-802C-767D2081AE8F}" name="PARA JG" dataDxfId="82" totalsRowDxfId="81">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="97" totalsRowDxfId="96">
+    <tableColumn id="16" xr3:uid="{A3F60C5A-D316-497E-B0E4-A3F9BAD84525}" name="PARA ABRECAR" dataDxfId="80" totalsRowDxfId="79">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="91"/>
+    <tableColumn id="17" xr3:uid="{10CB3E58-1A46-4C24-BA4F-AC5B36B8FF91}" name="ESTADO DEL SERVICIO" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{8BFE1AAE-4E74-4C50-BDE1-0DB10D889E57}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="19" xr3:uid="{206EECE6-638F-4588-8E77-382586BB3883}" name="NOTAS " totalsRowFunction="count" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="84" dataDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{DDAE932D-094A-412C-ACB3-D50B4144C427}" name="Tabla1456789101112" displayName="Tabla1456789101112" ref="A1:S41" totalsRowCount="1" headerRowDxfId="67" dataDxfId="66">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4821,38 +4841,38 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="82" totalsRowDxfId="81"/>
-    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="80"/>
-    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="79"/>
-    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="78"/>
-    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="76" totalsRowDxfId="75" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="70"/>
-    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="69" totalsRowDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="66" totalsRowDxfId="65">
+    <tableColumn id="1" xr3:uid="{A4610472-FCCC-49A0-A01F-092A0D751A98}" name="FECHA" totalsRowLabel="Total" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{F9E90005-75E9-4DFD-BEDF-137ACD9E05E4}" name="DIRECCION" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{F27B45B3-7483-405C-8490-165648DB5719}" name="NOMBRE CLIENTE" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{0FACF2B2-755C-4F0C-BA8A-14DC07017FD9}" name="TORRE/APTO" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{00E06524-BE36-4FF3-976B-47960F284CE0}" name="SERVICIO REALIZADO" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{5E93EC92-00AD-4B71-80D9-5F0B68DA5499}" name="DOMICILIO" dataDxfId="59" totalsRowDxfId="58" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FF6104F0-B72E-428D-8D64-20449974A374}" name="VALOR SERVICIO" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="8" xr3:uid="{CBA086A4-170D-485A-BDFD-EA146BD0B019}" name="MATERIALES" dataDxfId="55"/>
+    <tableColumn id="9" xr3:uid="{21A2EE02-A6EA-4899-886D-AFD1BA8755C3}" name="VALOR MATERIALES" dataDxfId="54"/>
+    <tableColumn id="10" xr3:uid="{1D00EAAB-65B1-4167-A677-7DFEA1816D65}" name="IVA 19%" dataDxfId="53"/>
+    <tableColumn id="11" xr3:uid="{2009E649-7D60-4DDB-8525-08B12BD6FA59}" name="PORTERIA" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{54BC3D94-5458-4653-8053-00D38144E7B3}" name="FORMA DE PAGO " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{A1498961-0B31-4EC8-87A8-0CA896C0FA28}" name="TOTAL SERVICIO" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="64" totalsRowDxfId="63"/>
-    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="62" totalsRowDxfId="61">
+    <tableColumn id="14" xr3:uid="{DCA18CC6-6586-4991-B645-0EFDB3C671BA}" name="X50%/X25%" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{EBD3F72E-644C-4987-97C9-741E83FF57A3}" name="PARA JG" dataDxfId="45" totalsRowDxfId="44">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="60" totalsRowDxfId="59">
+    <tableColumn id="16" xr3:uid="{582650E7-2FDF-4443-B176-6BD13705FC6A}" name="PARA ABRECAR" dataDxfId="43" totalsRowDxfId="42">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="54"/>
+    <tableColumn id="17" xr3:uid="{C9C0844F-A579-409B-A3CA-4CABDCA9A7E7}" name="ESTADO DEL SERVICIO" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="18" xr3:uid="{9BE8DE12-7A02-496D-8A4C-CF6A0FC21298}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="19" xr3:uid="{D05F4CC4-F427-42DD-B60E-F5C5874B0A10}" name="NOTAS " totalsRowFunction="count" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{4DF269EC-EC4E-479C-AE4F-1A1087AFCEE8}" name="Tabla145678910111213" displayName="Tabla145678910111213" ref="A1:S41" totalsRowCount="1" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:S40" xr:uid="{3F2D5825-CFDA-4ADD-8BFF-F4D8F9B37467}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4875,31 +4895,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" xr3:uid="{5055830B-9862-472C-85F0-117E805E707D}" name="FECHA" totalsRowLabel="Total" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{689C0FB3-87A6-4631-B1F6-2F9FCAA7E7B1}" name="DIRECCION" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{C1D134A7-FB44-4236-BBB6-7369A781153D}" name="NOMBRE CLIENTE" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{BD93EBE9-5715-4A8F-8BCE-7ED7B4E1EE00}" name="TORRE/APTO" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{D8732EE5-4B90-470C-AF7D-A9E30BB207AC}" name="SERVICIO REALIZADO" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{AAF6961D-5DCD-413C-8B1C-ACEFB0A3CFD9}" name="DOMICILIO" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{65ABEA60-8C9B-41B7-A56F-8019CBE25FF3}" name="VALOR SERVICIO" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{37401935-4C50-4C18-9EE8-ACDC29848F03}" name="MATERIALES" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{A93E3FC1-DC4F-4F49-A038-306F3DB5A2D6}" name="VALOR MATERIALES" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{D4E56074-FD4E-417D-B429-880CC1DD6054}" name="IVA 19%" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{A07BC7C7-BC63-43A4-A1DF-7229BD46E6AD}" name="PORTERIA" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{2AFC385D-3407-49B7-BF00-60E625E847AA}" name="FORMA DE PAGO " dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{E2603AC2-0F91-4E56-9786-C317F0769BE6}" name="TOTAL SERVICIO" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="25" totalsRowDxfId="24">
+    <tableColumn id="14" xr3:uid="{FD5B7BBF-B716-48D2-B942-472BC782EC98}" name="X50%/X25%" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{7D676C93-BA72-46B0-9F8A-8787870D86D0}" name="PARA JG" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="23" totalsRowDxfId="22">
+    <tableColumn id="16" xr3:uid="{BE3B5891-889F-41B1-B172-6BB026E6D50C}" name="PARA ABRECAR" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{A5F392B8-0A11-4121-9E91-E628125AA82C}" name="ESTADO DEL SERVICIO" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{553C6916-0493-4196-B3C4-4AC2BD6C71D7}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{131F3898-DF9C-4BB0-BA07-9F2E882DFC9F}" name="NOTAS " totalsRowFunction="count" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5307,31 +5327,31 @@
     <filterColumn colId="18" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="146" totalsRowDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="145" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="144" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="143"/>
-    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="142" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="141" totalsRowDxfId="12" dataCellStyle="Millares"/>
-    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="140" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="139" totalsRowDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="138" totalsRowDxfId="9"/>
-    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="137" totalsRowDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="136" totalsRowDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="135"/>
-    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="134" totalsRowDxfId="6">
+    <tableColumn id="1" xr3:uid="{C2D31F11-B0BA-45D5-A040-55DD65048FCC}" name="FECHA" totalsRowLabel="Total" dataDxfId="146" totalsRowDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{B04728B5-7F2E-44D9-B119-EB74F66021FF}" name="DIRECCION" dataDxfId="144" totalsRowDxfId="143"/>
+    <tableColumn id="3" xr3:uid="{34B0BF1B-1E1D-4372-8717-57CDDED3EB64}" name="NOMBRE CLIENTE" dataDxfId="142" totalsRowDxfId="141"/>
+    <tableColumn id="4" xr3:uid="{967AF0A4-2F6B-4902-9EE6-06F9B0ACEC7A}" name="TORRE/APTO" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{B7841EF7-1A13-48C8-9A8F-D8ECA1354F32}" name="SERVICIO REALIZADO" dataDxfId="139" totalsRowDxfId="138"/>
+    <tableColumn id="6" xr3:uid="{A5BD60C3-0F5D-4F7B-93D1-EAD5F5FF1B0B}" name="DOMICILIO" dataDxfId="137" totalsRowDxfId="136" dataCellStyle="Millares"/>
+    <tableColumn id="7" xr3:uid="{FE128F0E-0F30-41E9-92BC-73866EC54093}" name="VALOR SERVICIO" dataDxfId="135" totalsRowDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{DBFFBE5A-0B3E-47AA-B221-A8BE3A93FA28}" name="MATERIALES" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="9" xr3:uid="{E9AB51AF-E4E3-40DA-AB54-3DB3F1C528DD}" name="VALOR MATERIALES" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="10" xr3:uid="{0743077C-2C9E-4460-A4B5-D885E65A0FDD}" name="IVA 19%" dataDxfId="129" totalsRowDxfId="128"/>
+    <tableColumn id="11" xr3:uid="{5A1B6F72-1F83-47CD-8CB7-E840972ECC16}" name="PORTERIA" dataDxfId="127" totalsRowDxfId="126"/>
+    <tableColumn id="12" xr3:uid="{85785C1E-0B1B-4AE4-9899-F57CBFBDFCAB}" name="FORMA DE PAGO " dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{14E1E447-46F1-4DAB-8DAF-E7F4E090CDF7}" name="TOTAL SERVICIO" dataDxfId="124" totalsRowDxfId="123">
       <calculatedColumnFormula>(F2+G2-I2-K2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="133" totalsRowDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="132" totalsRowDxfId="4">
+    <tableColumn id="14" xr3:uid="{D122C8FB-7087-4CB5-A785-D8505B2DF602}" name="X50%/X25%" dataDxfId="122" totalsRowDxfId="121"/>
+    <tableColumn id="15" xr3:uid="{3B9C0FF4-0A40-425E-AF56-D6DD8681A011}" name="PARA JG" dataDxfId="120" totalsRowDxfId="119">
       <calculatedColumnFormula>IF(N2="X25%",M2*0.25,IF(N2="X50%",M2/2,""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="131" totalsRowDxfId="3">
+    <tableColumn id="16" xr3:uid="{24D7D408-20DD-481D-ADD8-31427D9706CB}" name="PARA ABRECAR" dataDxfId="118" totalsRowDxfId="117">
       <calculatedColumnFormula>(M2/2+J2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="130" totalsRowDxfId="2"/>
-    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="129" totalsRowDxfId="1"/>
-    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="128" totalsRowDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{3E22CA66-02BA-4F3A-BC78-1C5E81DF6614}" name="ESTADO DEL SERVICIO" dataDxfId="116" totalsRowDxfId="115"/>
+    <tableColumn id="18" xr3:uid="{BC2DF013-F795-4D1C-9028-1375AF4523CB}" name="FECHA DE RELACION DEL SERVICIO" dataDxfId="114" totalsRowDxfId="113"/>
+    <tableColumn id="19" xr3:uid="{72057D85-7D90-4121-8CBD-7448786FF9BC}" name="NOTAS " totalsRowFunction="count" dataDxfId="112" totalsRowDxfId="111"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8668,22 +8688,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="127" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="110" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="109" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="108" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="124" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="107" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="123" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="106" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="122" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9977,22 +9997,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="90" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="72" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11286,22 +11306,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:S41">
-    <cfRule type="expression" dxfId="53" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="1" stopIfTrue="1">
       <formula>$Q2="YA RELACIONADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="2" stopIfTrue="1">
       <formula>$Q2="COTIZACIÓN"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="3" stopIfTrue="1">
       <formula>$Q2="NO PAGARON DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
       <formula>$Q2="NO SE COBRA DOMICILIO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
       <formula>$Q2="GARANTIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
       <formula>$Q2="CANCELADO"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23639,8 +23659,8 @@
   </sheetPr>
   <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R11" sqref="R10:R11"/>
+    <sheetView tabSelected="1" topLeftCell="L4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24217,30 +24237,46 @@
         <v>670</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="14"/>
-      <c r="G11" s="17"/>
+    <row r="11" spans="1:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>45918</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>672</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>673</v>
+      </c>
+      <c r="G11" s="17">
+        <v>180000</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="17"/>
       <c r="J11" s="17"/>
       <c r="K11" s="6"/>
-      <c r="L11" s="14"/>
+      <c r="L11" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="M11" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="14"/>
-      <c r="O11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <v>180000</v>
+      </c>
+      <c r="N11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="1"/>
+        <v>90000</v>
       </c>
       <c r="P11" s="6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Q11" s="14"/>
       <c r="R11" s="2"/>

</xml_diff>